<commit_message>
Add sole titanium data
</commit_message>
<xml_diff>
--- a/static/mock/AntiBio1.xlsx
+++ b/static/mock/AntiBio1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/PycharmProjects/ChemML/static/mock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB07E97-7464-2A48-A7BB-A27307A4F7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2FA384-5CEB-B04E-AF06-7B62D8BA2668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{C97C895C-21C5-4ABD-B085-E1322DB1066B}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{C97C895C-21C5-4ABD-B085-E1322DB1066B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="203">
   <si>
     <t>RE</t>
   </si>
@@ -602,12 +602,6 @@
     <t>Shigella.dysenteriae</t>
   </si>
   <si>
-    <t>cRE, отн. Ед</t>
-  </si>
-  <si>
-    <t>КЧ2</t>
-  </si>
-  <si>
     <t>400.32</t>
   </si>
   <si>
@@ -683,9 +677,6 @@
     <t>Is_Salt</t>
   </si>
   <si>
-    <t xml:space="preserve">Stunting diameter </t>
-  </si>
-  <si>
     <t>Membrane pore diameter min</t>
   </si>
   <si>
@@ -702,6 +693,27 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Stunting diameter</t>
+  </si>
+  <si>
+    <t>REE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ionic_radii </t>
+  </si>
+  <si>
+    <t>electronegativity</t>
+  </si>
+  <si>
+    <t>crystal_structure_type</t>
+  </si>
+  <si>
+    <t>coordination_number_salt</t>
+  </si>
+  <si>
+    <t>coordination_number_solution</t>
   </si>
 </sst>
 </file>
@@ -1119,37 +1131,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1480,12 +1492,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2D3940D9-BD75-417D-B939-9D9F2B046451}" name="TLantTest" displayName="TLantTest" ref="A1:J17" totalsRowShown="0" dataDxfId="20">
   <autoFilter ref="A1:J17" xr:uid="{2D3940D9-BD75-417D-B939-9D9F2B046451}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{6E3D35CA-3D70-45F1-9A50-18CBC54E9741}" name="RE" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{48794F88-A244-474D-A6B2-9FD63736CE7C}" name="rRE, (VI),Ǻ1" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{DDE4413E-B094-4AFB-8138-A9932CA5D9D5}" name="cRE, отн. Ед" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{CFF1D428-BCF1-46DF-ACB8-4EBDDD164153}" name="СТ" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{0CA5AF80-08A7-4ED3-B39B-40669072521C}" name="КЧ" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{7FF2FE3D-DBC7-4F57-8794-C0C32F373CE2}" name="КЧ2" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{6E3D35CA-3D70-45F1-9A50-18CBC54E9741}" name="REE" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{48794F88-A244-474D-A6B2-9FD63736CE7C}" name="ionic_radii " dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{DDE4413E-B094-4AFB-8138-A9932CA5D9D5}" name="electronegativity" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{CFF1D428-BCF1-46DF-ACB8-4EBDDD164153}" name="crystal_structure_type" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{0CA5AF80-08A7-4ED3-B39B-40669072521C}" name="coordination_number_salt" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{7FF2FE3D-DBC7-4F57-8794-C0C32F373CE2}" name="coordination_number_solution" dataDxfId="14"/>
     <tableColumn id="7" xr3:uid="{3D5263EB-1B80-41C2-A1C6-35780FE385CD}" name="рН" dataDxfId="13"/>
     <tableColumn id="8" xr3:uid="{706A363A-7093-4406-B661-54FFDBA06FE1}" name="lgβ" dataDxfId="12"/>
     <tableColumn id="9" xr3:uid="{0FBAAE01-3DD2-4C00-AB7B-8504825C4F0D}" name="Electronic structure RE3+" dataDxfId="11"/>
@@ -1524,7 +1536,7 @@
     <tableColumn id="1" xr3:uid="{858DE136-ED7D-8F41-B550-768E6C966C6F}" name="RE" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{77255B40-8DC1-3845-9724-E04D52CFAA47}" name="Bacteria" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{0C923B2D-D05B-9D4F-BD93-17B59A424B0D}" name="Is_Salt"/>
-    <tableColumn id="4" xr3:uid="{55A8F227-AE1B-FF4C-8C62-9E53B05B48AF}" name="Stunting diameter "/>
+    <tableColumn id="4" xr3:uid="{55A8F227-AE1B-FF4C-8C62-9E53B05B48AF}" name="Stunting diameter"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1861,7 +1873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A1518FF-D6BA-47E6-9A12-FBC4CFEE5106}">
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="A48" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -1881,17 +1893,17 @@
       <c r="F1" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41" t="s">
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2053,35 +2065,35 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="34">
         <v>1.03</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="34">
         <v>2.4900000000000002</v>
       </c>
-      <c r="D6" s="33">
-        <v>1</v>
-      </c>
-      <c r="E6" s="33">
+      <c r="D6" s="34">
+        <v>1</v>
+      </c>
+      <c r="E6" s="34">
         <v>11</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="34">
         <v>11</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="34">
         <v>4.4400000000000004</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="33">
+      <c r="I6" s="34">
         <v>0.8</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="37">
         <v>138000</v>
       </c>
       <c r="L6" s="13" t="s">
@@ -2107,17 +2119,17 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="37"/>
       <c r="L7" s="13" t="s">
         <v>6</v>
       </c>
@@ -2141,17 +2153,17 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="13" t="s">
         <v>7</v>
       </c>
@@ -2175,17 +2187,17 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="37"/>
       <c r="L9" s="13" t="s">
         <v>8</v>
       </c>
@@ -2209,17 +2221,17 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="25"/>
       <c r="M10" s="3" t="s">
         <v>13</v>
@@ -2241,35 +2253,35 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="34">
         <v>1.01</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="34">
         <v>2.61</v>
       </c>
-      <c r="D11" s="33">
-        <v>1</v>
-      </c>
-      <c r="E11" s="33">
+      <c r="D11" s="34">
+        <v>1</v>
+      </c>
+      <c r="E11" s="34">
         <v>11</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="34">
         <v>11</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="34">
         <v>4.2</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="33">
+      <c r="I11" s="34">
         <v>0.9</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="34">
         <v>601.42999999999995</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="37">
         <v>32790</v>
       </c>
       <c r="L11" s="13" t="s">
@@ -2295,17 +2307,17 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="13" t="s">
         <v>16</v>
       </c>
@@ -2329,17 +2341,17 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="37"/>
       <c r="L13" s="13" t="s">
         <v>17</v>
       </c>
@@ -2363,17 +2375,17 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="13" t="s">
         <v>7</v>
       </c>
@@ -2397,17 +2409,17 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="37"/>
       <c r="L15" s="13" t="s">
         <v>8</v>
       </c>
@@ -2455,35 +2467,35 @@
       <c r="R16" s="14"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="34">
         <v>0.99</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="34">
         <v>2.2400000000000002</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="34">
         <v>2</v>
       </c>
-      <c r="E17" s="33">
-        <v>10</v>
-      </c>
-      <c r="F17" s="33">
-        <v>10</v>
-      </c>
-      <c r="G17" s="33">
+      <c r="E17" s="34">
+        <v>10</v>
+      </c>
+      <c r="F17" s="34">
+        <v>10</v>
+      </c>
+      <c r="G17" s="34">
         <v>4.51</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="33">
+      <c r="I17" s="34">
         <v>0.9</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="34">
         <v>602.42999999999995</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="37">
         <v>98500</v>
       </c>
       <c r="L17" s="13" t="s">
@@ -2504,20 +2516,20 @@
       <c r="Q17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R17" s="36"/>
+      <c r="R17" s="39"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="37"/>
       <c r="L18" s="13" t="s">
         <v>16</v>
       </c>
@@ -2536,20 +2548,20 @@
       <c r="Q18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R18" s="36"/>
+      <c r="R18" s="39"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="35"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="37"/>
       <c r="L19" s="13" t="s">
         <v>17</v>
       </c>
@@ -2568,20 +2580,20 @@
       <c r="Q19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R19" s="36"/>
+      <c r="R19" s="39"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="35"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="37"/>
       <c r="L20" s="13" t="s">
         <v>7</v>
       </c>
@@ -2600,20 +2612,20 @@
       <c r="Q20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R20" s="36"/>
+      <c r="R20" s="39"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="35"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="37"/>
       <c r="L21" s="13" t="s">
         <v>8</v>
       </c>
@@ -2632,38 +2644,38 @@
       <c r="Q21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R21" s="36"/>
+      <c r="R21" s="39"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="33">
+      <c r="B22" s="34">
         <v>0.96</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C22" s="34">
         <v>1.9</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="34">
         <v>2</v>
       </c>
-      <c r="E22" s="33">
-        <v>10</v>
-      </c>
-      <c r="F22" s="33">
-        <v>10</v>
-      </c>
-      <c r="G22" s="33">
+      <c r="E22" s="34">
+        <v>10</v>
+      </c>
+      <c r="F22" s="34">
+        <v>10</v>
+      </c>
+      <c r="G22" s="34">
         <v>5.08</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="33">
+      <c r="I22" s="34">
         <v>0.9</v>
       </c>
-      <c r="J22" s="33">
+      <c r="J22" s="34">
         <v>602.43299999999999</v>
       </c>
-      <c r="K22" s="34">
+      <c r="K22" s="37">
         <v>97000</v>
       </c>
       <c r="L22" s="13" t="s">
@@ -2689,17 +2701,17 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="35"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="37"/>
       <c r="L23" s="13" t="s">
         <v>16</v>
       </c>
@@ -2723,17 +2735,17 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="35"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="37"/>
       <c r="L24" s="13" t="s">
         <v>17</v>
       </c>
@@ -2757,17 +2769,17 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="35"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="37"/>
       <c r="L25" s="13" t="s">
         <v>7</v>
       </c>
@@ -2791,17 +2803,17 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="37"/>
       <c r="L26" s="13" t="s">
         <v>8</v>
       </c>
@@ -2825,35 +2837,35 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="33">
+      <c r="B27" s="34">
         <v>0.95</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="34">
         <v>1.81</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="34">
         <v>2</v>
       </c>
-      <c r="E27" s="33">
-        <v>10</v>
-      </c>
-      <c r="F27" s="33">
-        <v>10</v>
-      </c>
-      <c r="G27" s="33">
+      <c r="E27" s="34">
+        <v>10</v>
+      </c>
+      <c r="F27" s="34">
+        <v>10</v>
+      </c>
+      <c r="G27" s="34">
         <v>5.56</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="33">
+      <c r="I27" s="34">
         <v>0.8</v>
       </c>
-      <c r="J27" s="33">
+      <c r="J27" s="34">
         <v>602.43399999999997</v>
       </c>
-      <c r="K27" s="34">
+      <c r="K27" s="37">
         <v>134500</v>
       </c>
       <c r="L27" s="13" t="s">
@@ -2874,20 +2886,20 @@
       <c r="Q27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R27" s="36"/>
+      <c r="R27" s="39"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="37"/>
       <c r="L28" s="13" t="s">
         <v>16</v>
       </c>
@@ -2906,20 +2918,20 @@
       <c r="Q28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R28" s="36"/>
+      <c r="R28" s="39"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="37"/>
       <c r="L29" s="13" t="s">
         <v>17</v>
       </c>
@@ -2938,20 +2950,20 @@
       <c r="Q29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R29" s="36"/>
+      <c r="R29" s="39"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="35"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="37"/>
       <c r="L30" s="13" t="s">
         <v>7</v>
       </c>
@@ -2970,20 +2982,20 @@
       <c r="Q30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R30" s="36"/>
+      <c r="R30" s="39"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="35"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="37"/>
       <c r="L31" s="13" t="s">
         <v>8</v>
       </c>
@@ -3002,38 +3014,38 @@
       <c r="Q31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R31" s="36"/>
+      <c r="R31" s="39"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="33">
+      <c r="B32" s="34">
         <v>0.94</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="34">
         <v>2.4</v>
       </c>
-      <c r="D32" s="33">
+      <c r="D32" s="34">
         <v>2</v>
       </c>
-      <c r="E32" s="33">
-        <v>10</v>
-      </c>
-      <c r="F32" s="33">
-        <v>10</v>
-      </c>
-      <c r="G32" s="33">
+      <c r="E32" s="34">
+        <v>10</v>
+      </c>
+      <c r="F32" s="34">
+        <v>10</v>
+      </c>
+      <c r="G32" s="34">
         <v>4.51</v>
       </c>
       <c r="H32" s="3"/>
-      <c r="I32" s="33">
+      <c r="I32" s="34">
         <v>0.8</v>
       </c>
-      <c r="J32" s="33" t="s">
+      <c r="J32" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="K32" s="34">
+      <c r="K32" s="37">
         <v>78450</v>
       </c>
       <c r="L32" s="13" t="s">
@@ -3059,17 +3071,17 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" s="35"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="37"/>
       <c r="L33" s="13" t="s">
         <v>16</v>
       </c>
@@ -3093,17 +3105,17 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A34" s="35"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="37"/>
       <c r="L34" s="13" t="s">
         <v>17</v>
       </c>
@@ -3127,17 +3139,17 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A35" s="35"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="37"/>
       <c r="L35" s="13" t="s">
         <v>7</v>
       </c>
@@ -3161,17 +3173,17 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" s="35"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="37"/>
       <c r="L36" s="13" t="s">
         <v>8</v>
       </c>
@@ -3195,35 +3207,35 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="33">
+      <c r="B37" s="34">
         <v>0.92</v>
       </c>
-      <c r="C37" s="33">
+      <c r="C37" s="34">
         <v>2.29</v>
       </c>
-      <c r="D37" s="33">
+      <c r="D37" s="34">
         <v>2</v>
       </c>
-      <c r="E37" s="33">
-        <v>10</v>
-      </c>
-      <c r="F37" s="33">
-        <v>10</v>
-      </c>
-      <c r="G37" s="33">
+      <c r="E37" s="34">
+        <v>10</v>
+      </c>
+      <c r="F37" s="34">
+        <v>10</v>
+      </c>
+      <c r="G37" s="34">
         <v>1.87</v>
       </c>
       <c r="H37" s="3"/>
-      <c r="I37" s="33">
+      <c r="I37" s="34">
         <v>0.7</v>
       </c>
-      <c r="J37" s="33">
+      <c r="J37" s="34">
         <v>602.43600000000004</v>
       </c>
-      <c r="K37" s="34">
+      <c r="K37" s="37">
         <v>81650</v>
       </c>
       <c r="L37" s="13" t="s">
@@ -3244,20 +3256,20 @@
       <c r="Q37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R37" s="36"/>
+      <c r="R37" s="39"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" s="35"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="37"/>
       <c r="L38" s="13" t="s">
         <v>16</v>
       </c>
@@ -3276,20 +3288,20 @@
       <c r="Q38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R38" s="36"/>
+      <c r="R38" s="39"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="35"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="37"/>
       <c r="L39" s="13" t="s">
         <v>17</v>
       </c>
@@ -3308,20 +3320,20 @@
       <c r="Q39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R39" s="36"/>
+      <c r="R39" s="39"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" s="35"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="37"/>
       <c r="L40" s="13" t="s">
         <v>7</v>
       </c>
@@ -3340,20 +3352,20 @@
       <c r="Q40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R40" s="36"/>
+      <c r="R40" s="39"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A41" s="35"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="37"/>
       <c r="L41" s="13" t="s">
         <v>8</v>
       </c>
@@ -3372,38 +3384,38 @@
       <c r="Q41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R41" s="36"/>
+      <c r="R41" s="39"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="33">
+      <c r="B42" s="34">
         <v>0.91</v>
       </c>
-      <c r="C42" s="33">
+      <c r="C42" s="34">
         <v>2.0699999999999998</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D42" s="34">
         <v>3</v>
       </c>
-      <c r="E42" s="33">
-        <v>10</v>
-      </c>
-      <c r="F42" s="33">
-        <v>10</v>
-      </c>
-      <c r="G42" s="33">
+      <c r="E42" s="34">
+        <v>10</v>
+      </c>
+      <c r="F42" s="34">
+        <v>10</v>
+      </c>
+      <c r="G42" s="34">
         <v>5.78</v>
       </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="33">
+      <c r="I42" s="34">
         <v>0.6</v>
       </c>
-      <c r="J42" s="33">
+      <c r="J42" s="34">
         <v>602.43700000000001</v>
       </c>
-      <c r="K42" s="34">
+      <c r="K42" s="37">
         <v>72000</v>
       </c>
       <c r="L42" s="13" t="s">
@@ -3424,20 +3436,20 @@
       <c r="Q42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R42" s="36"/>
+      <c r="R42" s="39"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" s="35"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
+      <c r="K43" s="37"/>
       <c r="L43" s="13" t="s">
         <v>16</v>
       </c>
@@ -3456,20 +3468,20 @@
       <c r="Q43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R43" s="36"/>
+      <c r="R43" s="39"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A44" s="35"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="37"/>
       <c r="L44" s="13" t="s">
         <v>17</v>
       </c>
@@ -3488,20 +3500,20 @@
       <c r="Q44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R44" s="36"/>
+      <c r="R44" s="39"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="35"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="37"/>
       <c r="L45" s="13" t="s">
         <v>7</v>
       </c>
@@ -3520,20 +3532,20 @@
       <c r="Q45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R45" s="36"/>
+      <c r="R45" s="39"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="35"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="37"/>
       <c r="L46" s="13" t="s">
         <v>8</v>
       </c>
@@ -3552,38 +3564,38 @@
       <c r="Q46" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R46" s="36"/>
+      <c r="R46" s="39"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="33">
+      <c r="B47" s="34">
         <v>0.9</v>
       </c>
-      <c r="C47" s="33">
+      <c r="C47" s="34">
         <v>2.12</v>
       </c>
-      <c r="D47" s="33">
+      <c r="D47" s="34">
         <v>3</v>
       </c>
-      <c r="E47" s="33">
+      <c r="E47" s="34">
         <v>9</v>
       </c>
-      <c r="F47" s="33">
+      <c r="F47" s="34">
         <v>9</v>
       </c>
-      <c r="G47" s="33">
+      <c r="G47" s="34">
         <v>5.96</v>
       </c>
       <c r="H47" s="3"/>
-      <c r="I47" s="33">
+      <c r="I47" s="34">
         <v>0.5</v>
       </c>
-      <c r="J47" s="33">
+      <c r="J47" s="34">
         <v>602.43799999999999</v>
       </c>
-      <c r="K47" s="34">
+      <c r="K47" s="37">
         <v>16000</v>
       </c>
       <c r="L47" s="13" t="s">
@@ -3595,23 +3607,23 @@
       <c r="N47" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="O47" s="37"/>
-      <c r="P47" s="33"/>
-      <c r="Q47" s="33"/>
-      <c r="R47" s="36"/>
+      <c r="O47" s="43"/>
+      <c r="P47" s="34"/>
+      <c r="Q47" s="34"/>
+      <c r="R47" s="39"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A48" s="35"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
+      <c r="A48" s="41"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="37"/>
       <c r="L48" s="13" t="s">
         <v>16</v>
       </c>
@@ -3621,23 +3633,23 @@
       <c r="N48" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="O48" s="37"/>
-      <c r="P48" s="33"/>
-      <c r="Q48" s="33"/>
-      <c r="R48" s="36"/>
+      <c r="O48" s="43"/>
+      <c r="P48" s="34"/>
+      <c r="Q48" s="34"/>
+      <c r="R48" s="39"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" s="35"/>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="34"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="37"/>
       <c r="L49" s="13" t="s">
         <v>17</v>
       </c>
@@ -3647,23 +3659,23 @@
       <c r="N49" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="O49" s="37"/>
-      <c r="P49" s="33"/>
-      <c r="Q49" s="33"/>
-      <c r="R49" s="36"/>
+      <c r="O49" s="43"/>
+      <c r="P49" s="34"/>
+      <c r="Q49" s="34"/>
+      <c r="R49" s="39"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A50" s="35"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="37"/>
       <c r="L50" s="13" t="s">
         <v>7</v>
       </c>
@@ -3673,23 +3685,23 @@
       <c r="N50" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="O50" s="37"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="33"/>
-      <c r="R50" s="36"/>
+      <c r="O50" s="43"/>
+      <c r="P50" s="34"/>
+      <c r="Q50" s="34"/>
+      <c r="R50" s="39"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A51" s="35"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
+      <c r="A51" s="41"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="34"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="34"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="37"/>
       <c r="L51" s="13" t="s">
         <v>8</v>
       </c>
@@ -3699,41 +3711,41 @@
       <c r="N51" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O51" s="37"/>
-      <c r="P51" s="33"/>
-      <c r="Q51" s="33"/>
-      <c r="R51" s="36"/>
+      <c r="O51" s="43"/>
+      <c r="P51" s="34"/>
+      <c r="Q51" s="34"/>
+      <c r="R51" s="39"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="33">
+      <c r="B52" s="34">
         <v>0.89</v>
       </c>
-      <c r="C52" s="33">
+      <c r="C52" s="34">
         <v>2.02</v>
       </c>
-      <c r="D52" s="33">
+      <c r="D52" s="34">
         <v>4</v>
       </c>
-      <c r="E52" s="33">
+      <c r="E52" s="34">
         <v>9</v>
       </c>
-      <c r="F52" s="33">
+      <c r="F52" s="34">
         <v>9</v>
       </c>
-      <c r="G52" s="33">
+      <c r="G52" s="34">
         <v>5.16</v>
       </c>
       <c r="H52" s="3"/>
-      <c r="I52" s="33">
+      <c r="I52" s="34">
         <v>0.4</v>
       </c>
-      <c r="J52" s="33">
+      <c r="J52" s="34">
         <v>602.43899999999996</v>
       </c>
-      <c r="K52" s="34">
+      <c r="K52" s="37">
         <v>89500</v>
       </c>
       <c r="L52" s="13" t="s">
@@ -3754,20 +3766,20 @@
       <c r="Q52" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R52" s="36"/>
+      <c r="R52" s="39"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A53" s="35"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
+      <c r="A53" s="41"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="33"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="37"/>
       <c r="L53" s="13" t="s">
         <v>16</v>
       </c>
@@ -3786,20 +3798,20 @@
       <c r="Q53" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R53" s="36"/>
+      <c r="R53" s="39"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="35"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
+      <c r="A54" s="41"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="33"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="34"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="34"/>
+      <c r="K54" s="37"/>
       <c r="L54" s="13" t="s">
         <v>17</v>
       </c>
@@ -3818,20 +3830,20 @@
       <c r="Q54" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R54" s="36"/>
+      <c r="R54" s="39"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="35"/>
-      <c r="B55" s="33"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
+      <c r="A55" s="41"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="33"/>
-      <c r="J55" s="33"/>
-      <c r="K55" s="34"/>
+      <c r="I55" s="34"/>
+      <c r="J55" s="34"/>
+      <c r="K55" s="37"/>
       <c r="L55" s="13" t="s">
         <v>7</v>
       </c>
@@ -3850,20 +3862,20 @@
       <c r="Q55" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R55" s="36"/>
+      <c r="R55" s="39"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="35"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
+      <c r="A56" s="41"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="33"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="34"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="37"/>
       <c r="L56" s="13" t="s">
         <v>8</v>
       </c>
@@ -3882,38 +3894,38 @@
       <c r="Q56" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R56" s="36"/>
+      <c r="R56" s="39"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="33">
+      <c r="B57" s="34">
         <v>0.88</v>
       </c>
-      <c r="C57" s="33">
+      <c r="C57" s="34">
         <v>2.0299999999999998</v>
       </c>
-      <c r="D57" s="33">
+      <c r="D57" s="34">
         <v>4</v>
       </c>
-      <c r="E57" s="33">
+      <c r="E57" s="34">
         <v>9</v>
       </c>
-      <c r="F57" s="33">
+      <c r="F57" s="34">
         <v>9</v>
       </c>
-      <c r="G57" s="33">
+      <c r="G57" s="34">
         <v>5.54</v>
       </c>
       <c r="H57" s="3"/>
-      <c r="I57" s="33">
+      <c r="I57" s="34">
         <v>0.4</v>
       </c>
-      <c r="J57" s="33">
+      <c r="J57" s="34">
         <v>602.43100000000004</v>
       </c>
-      <c r="K57" s="34">
+      <c r="K57" s="37">
         <v>44910</v>
       </c>
       <c r="L57" s="13" t="s">
@@ -3934,20 +3946,20 @@
       <c r="Q57" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R57" s="36"/>
+      <c r="R57" s="39"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="35"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
+      <c r="A58" s="41"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="37"/>
       <c r="L58" s="13" t="s">
         <v>16</v>
       </c>
@@ -3966,20 +3978,20 @@
       <c r="Q58" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R58" s="36"/>
+      <c r="R58" s="39"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A59" s="35"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
+      <c r="A59" s="41"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="34"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="37"/>
       <c r="L59" s="13" t="s">
         <v>17</v>
       </c>
@@ -3998,20 +4010,20 @@
       <c r="Q59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R59" s="36"/>
+      <c r="R59" s="39"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="35"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
+      <c r="A60" s="41"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="37"/>
       <c r="L60" s="13" t="s">
         <v>7</v>
       </c>
@@ -4030,20 +4042,20 @@
       <c r="Q60" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R60" s="36"/>
+      <c r="R60" s="39"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="35"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
+      <c r="A61" s="41"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="34"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="37"/>
       <c r="L61" s="13" t="s">
         <v>8</v>
       </c>
@@ -4062,38 +4074,38 @@
       <c r="Q61" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R61" s="36"/>
+      <c r="R61" s="39"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="33">
+      <c r="B62" s="34">
         <v>0.87</v>
       </c>
-      <c r="C62" s="33">
+      <c r="C62" s="34">
         <v>1.78</v>
       </c>
-      <c r="D62" s="33">
+      <c r="D62" s="34">
         <v>5</v>
       </c>
-      <c r="E62" s="33">
+      <c r="E62" s="34">
         <v>9</v>
       </c>
-      <c r="F62" s="33">
+      <c r="F62" s="34">
         <v>9</v>
       </c>
-      <c r="G62" s="33">
+      <c r="G62" s="34">
         <v>5.74</v>
       </c>
       <c r="H62" s="3"/>
-      <c r="I62" s="33">
+      <c r="I62" s="34">
         <v>0.4</v>
       </c>
-      <c r="J62" s="33" t="s">
+      <c r="J62" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="K62" s="34">
+      <c r="K62" s="37">
         <v>84040</v>
       </c>
       <c r="L62" s="13" t="s">
@@ -4119,17 +4131,17 @@
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="35"/>
-      <c r="B63" s="33"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
+      <c r="A63" s="41"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="34"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="34"/>
+      <c r="I63" s="34"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="37"/>
       <c r="L63" s="13" t="s">
         <v>16</v>
       </c>
@@ -4153,17 +4165,17 @@
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="35"/>
-      <c r="B64" s="33"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="33"/>
-      <c r="F64" s="33"/>
-      <c r="G64" s="33"/>
+      <c r="A64" s="41"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="33"/>
-      <c r="J64" s="33"/>
-      <c r="K64" s="34"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="37"/>
       <c r="L64" s="13" t="s">
         <v>17</v>
       </c>
@@ -4187,17 +4199,17 @@
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A65" s="35"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
+      <c r="A65" s="41"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="34"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="33"/>
-      <c r="J65" s="33"/>
-      <c r="K65" s="34"/>
+      <c r="I65" s="34"/>
+      <c r="J65" s="34"/>
+      <c r="K65" s="37"/>
       <c r="L65" s="13" t="s">
         <v>7</v>
       </c>
@@ -4221,17 +4233,17 @@
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A66" s="35"/>
-      <c r="B66" s="33"/>
-      <c r="C66" s="33"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="33"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="33"/>
+      <c r="A66" s="41"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="33"/>
-      <c r="J66" s="33"/>
-      <c r="K66" s="34"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="37"/>
       <c r="L66" s="13" t="s">
         <v>8</v>
       </c>
@@ -4255,35 +4267,35 @@
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="33">
+      <c r="B67" s="34">
         <v>0.86</v>
       </c>
-      <c r="C67" s="33">
+      <c r="C67" s="34">
         <v>2.68</v>
       </c>
-      <c r="D67" s="33">
+      <c r="D67" s="34">
         <v>7</v>
       </c>
-      <c r="E67" s="33">
+      <c r="E67" s="34">
         <v>9</v>
       </c>
-      <c r="F67" s="33">
+      <c r="F67" s="34">
         <v>9</v>
       </c>
-      <c r="G67" s="33">
+      <c r="G67" s="34">
         <v>5.5</v>
       </c>
       <c r="H67" s="3"/>
-      <c r="I67" s="33">
+      <c r="I67" s="34">
         <v>0.6</v>
       </c>
-      <c r="J67" s="33" t="s">
+      <c r="J67" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="K67" s="34">
+      <c r="K67" s="37">
         <v>252000</v>
       </c>
       <c r="L67" s="13" t="s">
@@ -4304,20 +4316,20 @@
       <c r="Q67" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="R67" s="36"/>
+      <c r="R67" s="39"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A68" s="35"/>
-      <c r="B68" s="33"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="33"/>
-      <c r="E68" s="33"/>
-      <c r="F68" s="33"/>
-      <c r="G68" s="33"/>
+      <c r="A68" s="41"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="34"/>
+      <c r="G68" s="34"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="33"/>
-      <c r="J68" s="33"/>
-      <c r="K68" s="34"/>
+      <c r="I68" s="34"/>
+      <c r="J68" s="34"/>
+      <c r="K68" s="37"/>
       <c r="L68" s="13" t="s">
         <v>16</v>
       </c>
@@ -4336,20 +4348,20 @@
       <c r="Q68" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R68" s="36"/>
+      <c r="R68" s="39"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A69" s="35"/>
-      <c r="B69" s="33"/>
-      <c r="C69" s="33"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="33"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="33"/>
+      <c r="A69" s="41"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="33"/>
-      <c r="J69" s="33"/>
-      <c r="K69" s="34"/>
+      <c r="I69" s="34"/>
+      <c r="J69" s="34"/>
+      <c r="K69" s="37"/>
       <c r="L69" s="13" t="s">
         <v>17</v>
       </c>
@@ -4368,20 +4380,20 @@
       <c r="Q69" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R69" s="36"/>
+      <c r="R69" s="39"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A70" s="35"/>
-      <c r="B70" s="33"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="33"/>
+      <c r="A70" s="41"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="34"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="33"/>
-      <c r="J70" s="33"/>
-      <c r="K70" s="34"/>
+      <c r="I70" s="34"/>
+      <c r="J70" s="34"/>
+      <c r="K70" s="37"/>
       <c r="L70" s="13" t="s">
         <v>7</v>
       </c>
@@ -4400,20 +4412,20 @@
       <c r="Q70" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R70" s="36"/>
+      <c r="R70" s="39"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A71" s="35"/>
-      <c r="B71" s="33"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="33"/>
-      <c r="F71" s="33"/>
-      <c r="G71" s="33"/>
+      <c r="A71" s="41"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="34"/>
+      <c r="G71" s="34"/>
       <c r="H71" s="3"/>
-      <c r="I71" s="33"/>
-      <c r="J71" s="33"/>
-      <c r="K71" s="34"/>
+      <c r="I71" s="34"/>
+      <c r="J71" s="34"/>
+      <c r="K71" s="37"/>
       <c r="L71" s="13" t="s">
         <v>8</v>
       </c>
@@ -4432,38 +4444,38 @@
       <c r="Q71" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R71" s="36"/>
+      <c r="R71" s="39"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A72" s="35" t="s">
+      <c r="A72" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="33">
+      <c r="B72" s="34">
         <v>0.9</v>
       </c>
-      <c r="C72" s="33">
+      <c r="C72" s="34">
         <v>2.52</v>
       </c>
-      <c r="D72" s="33">
+      <c r="D72" s="34">
         <v>2</v>
       </c>
-      <c r="E72" s="33">
-        <v>10</v>
-      </c>
-      <c r="F72" s="33">
-        <v>10</v>
-      </c>
-      <c r="G72" s="33">
+      <c r="E72" s="34">
+        <v>10</v>
+      </c>
+      <c r="F72" s="34">
+        <v>10</v>
+      </c>
+      <c r="G72" s="34">
         <v>5.92</v>
       </c>
       <c r="H72" s="3"/>
-      <c r="I72" s="33">
+      <c r="I72" s="34">
         <v>0.4</v>
       </c>
-      <c r="J72" s="33">
+      <c r="J72" s="34">
         <v>500.42</v>
       </c>
-      <c r="K72" s="34">
+      <c r="K72" s="37">
         <v>15260</v>
       </c>
       <c r="L72" s="13" t="s">
@@ -4489,17 +4501,17 @@
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A73" s="35"/>
-      <c r="B73" s="33"/>
-      <c r="C73" s="33"/>
-      <c r="D73" s="33"/>
-      <c r="E73" s="33"/>
-      <c r="F73" s="33"/>
-      <c r="G73" s="33"/>
+      <c r="A73" s="41"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="34"/>
+      <c r="G73" s="34"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="33"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="34"/>
+      <c r="I73" s="34"/>
+      <c r="J73" s="34"/>
+      <c r="K73" s="37"/>
       <c r="L73" s="13" t="s">
         <v>16</v>
       </c>
@@ -4523,17 +4535,17 @@
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A74" s="35"/>
-      <c r="B74" s="33"/>
-      <c r="C74" s="33"/>
-      <c r="D74" s="33"/>
-      <c r="E74" s="33"/>
-      <c r="F74" s="33"/>
-      <c r="G74" s="33"/>
+      <c r="A74" s="41"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="34"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="33"/>
-      <c r="J74" s="33"/>
-      <c r="K74" s="34"/>
+      <c r="I74" s="34"/>
+      <c r="J74" s="34"/>
+      <c r="K74" s="37"/>
       <c r="L74" s="13" t="s">
         <v>17</v>
       </c>
@@ -4557,17 +4569,17 @@
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A75" s="35"/>
-      <c r="B75" s="33"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
+      <c r="A75" s="41"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="34"/>
+      <c r="G75" s="34"/>
       <c r="H75" s="3"/>
-      <c r="I75" s="33"/>
-      <c r="J75" s="33"/>
-      <c r="K75" s="34"/>
+      <c r="I75" s="34"/>
+      <c r="J75" s="34"/>
+      <c r="K75" s="37"/>
       <c r="L75" s="13" t="s">
         <v>7</v>
       </c>
@@ -4591,17 +4603,17 @@
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A76" s="35"/>
-      <c r="B76" s="33"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
+      <c r="A76" s="41"/>
+      <c r="B76" s="34"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="34"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="33"/>
-      <c r="J76" s="33"/>
-      <c r="K76" s="34"/>
+      <c r="I76" s="34"/>
+      <c r="J76" s="34"/>
+      <c r="K76" s="37"/>
       <c r="L76" s="13" t="s">
         <v>8</v>
       </c>
@@ -4625,33 +4637,33 @@
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A77" s="35" t="s">
+      <c r="A77" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B77" s="33">
+      <c r="B77" s="34">
         <v>0.75</v>
       </c>
-      <c r="C77" s="33">
+      <c r="C77" s="34">
         <v>2.35</v>
       </c>
-      <c r="D77" s="33">
+      <c r="D77" s="34">
         <v>6</v>
       </c>
-      <c r="E77" s="33">
+      <c r="E77" s="34">
         <v>6</v>
       </c>
-      <c r="F77" s="33">
+      <c r="F77" s="34">
         <v>6</v>
       </c>
-      <c r="G77" s="33">
+      <c r="G77" s="34">
         <v>2.0299999999999998</v>
       </c>
       <c r="H77" s="3"/>
-      <c r="I77" s="33"/>
-      <c r="J77" s="33">
+      <c r="I77" s="34"/>
+      <c r="J77" s="34">
         <v>400.32</v>
       </c>
-      <c r="K77" s="34">
+      <c r="K77" s="37">
         <v>286300</v>
       </c>
       <c r="L77" s="13" t="s">
@@ -4672,20 +4684,20 @@
       <c r="Q77" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R77" s="36"/>
+      <c r="R77" s="39"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A78" s="35"/>
-      <c r="B78" s="33"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="33"/>
+      <c r="A78" s="41"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="34"/>
+      <c r="G78" s="34"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="33"/>
-      <c r="J78" s="33"/>
-      <c r="K78" s="34"/>
+      <c r="I78" s="34"/>
+      <c r="J78" s="34"/>
+      <c r="K78" s="37"/>
       <c r="L78" s="13" t="s">
         <v>16</v>
       </c>
@@ -4704,20 +4716,20 @@
       <c r="Q78" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R78" s="36"/>
+      <c r="R78" s="39"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A79" s="35"/>
-      <c r="B79" s="33"/>
-      <c r="C79" s="33"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="33"/>
+      <c r="A79" s="41"/>
+      <c r="B79" s="34"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="34"/>
+      <c r="F79" s="34"/>
+      <c r="G79" s="34"/>
       <c r="H79" s="3"/>
-      <c r="I79" s="33"/>
-      <c r="J79" s="33"/>
-      <c r="K79" s="34"/>
+      <c r="I79" s="34"/>
+      <c r="J79" s="34"/>
+      <c r="K79" s="37"/>
       <c r="L79" s="13" t="s">
         <v>17</v>
       </c>
@@ -4736,20 +4748,20 @@
       <c r="Q79" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R79" s="36"/>
+      <c r="R79" s="39"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A80" s="35"/>
-      <c r="B80" s="33"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
+      <c r="A80" s="41"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
       <c r="H80" s="3"/>
-      <c r="I80" s="33"/>
-      <c r="J80" s="33"/>
-      <c r="K80" s="34"/>
+      <c r="I80" s="34"/>
+      <c r="J80" s="34"/>
+      <c r="K80" s="37"/>
       <c r="L80" s="13" t="s">
         <v>7</v>
       </c>
@@ -4768,20 +4780,20 @@
       <c r="Q80" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R80" s="36"/>
+      <c r="R80" s="39"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A81" s="35"/>
-      <c r="B81" s="33"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="33"/>
-      <c r="F81" s="33"/>
-      <c r="G81" s="33"/>
+      <c r="A81" s="41"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="34"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="34"/>
+      <c r="F81" s="34"/>
+      <c r="G81" s="34"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="33"/>
-      <c r="J81" s="33"/>
-      <c r="K81" s="34"/>
+      <c r="I81" s="34"/>
+      <c r="J81" s="34"/>
+      <c r="K81" s="37"/>
       <c r="L81" s="13" t="s">
         <v>8</v>
       </c>
@@ -4800,36 +4812,36 @@
       <c r="Q81" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R81" s="36"/>
+      <c r="R81" s="39"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A82" s="35" t="s">
+      <c r="A82" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B82" s="33">
-        <v>1</v>
-      </c>
-      <c r="C82" s="33">
+      <c r="B82" s="34">
+        <v>1</v>
+      </c>
+      <c r="C82" s="34">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D82" s="33">
+      <c r="D82" s="34">
         <v>7</v>
       </c>
-      <c r="E82" s="33">
+      <c r="E82" s="34">
         <v>6</v>
       </c>
-      <c r="F82" s="33">
+      <c r="F82" s="34">
         <v>6</v>
       </c>
-      <c r="G82" s="33">
+      <c r="G82" s="34">
         <v>5.63</v>
       </c>
       <c r="H82" s="3"/>
-      <c r="I82" s="33"/>
-      <c r="J82" s="33">
+      <c r="I82" s="34"/>
+      <c r="J82" s="34">
         <v>400</v>
       </c>
-      <c r="K82" s="34" t="s">
+      <c r="K82" s="37" t="s">
         <v>74</v>
       </c>
       <c r="L82" s="13" t="s">
@@ -4850,20 +4862,20 @@
       <c r="Q82" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R82" s="36"/>
+      <c r="R82" s="39"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A83" s="35"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="33"/>
-      <c r="F83" s="33"/>
-      <c r="G83" s="33"/>
+      <c r="A83" s="41"/>
+      <c r="B83" s="34"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="34"/>
+      <c r="G83" s="34"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="33"/>
-      <c r="J83" s="33"/>
-      <c r="K83" s="34"/>
+      <c r="I83" s="34"/>
+      <c r="J83" s="34"/>
+      <c r="K83" s="37"/>
       <c r="L83" s="13" t="s">
         <v>16</v>
       </c>
@@ -4882,20 +4894,20 @@
       <c r="Q83" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R83" s="36"/>
+      <c r="R83" s="39"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A84" s="35"/>
-      <c r="B84" s="33"/>
-      <c r="C84" s="33"/>
-      <c r="D84" s="33"/>
-      <c r="E84" s="33"/>
-      <c r="F84" s="33"/>
-      <c r="G84" s="33"/>
+      <c r="A84" s="41"/>
+      <c r="B84" s="34"/>
+      <c r="C84" s="34"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="34"/>
+      <c r="F84" s="34"/>
+      <c r="G84" s="34"/>
       <c r="H84" s="3"/>
-      <c r="I84" s="33"/>
-      <c r="J84" s="33"/>
-      <c r="K84" s="34"/>
+      <c r="I84" s="34"/>
+      <c r="J84" s="34"/>
+      <c r="K84" s="37"/>
       <c r="L84" s="13" t="s">
         <v>17</v>
       </c>
@@ -4914,20 +4926,20 @@
       <c r="Q84" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R84" s="36"/>
+      <c r="R84" s="39"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A85" s="35"/>
-      <c r="B85" s="33"/>
-      <c r="C85" s="33"/>
-      <c r="D85" s="33"/>
-      <c r="E85" s="33"/>
-      <c r="F85" s="33"/>
-      <c r="G85" s="33"/>
+      <c r="A85" s="41"/>
+      <c r="B85" s="34"/>
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="34"/>
+      <c r="G85" s="34"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="33"/>
-      <c r="J85" s="33"/>
-      <c r="K85" s="34"/>
+      <c r="I85" s="34"/>
+      <c r="J85" s="34"/>
+      <c r="K85" s="37"/>
       <c r="L85" s="13" t="s">
         <v>7</v>
       </c>
@@ -4946,20 +4958,20 @@
       <c r="Q85" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R85" s="36"/>
+      <c r="R85" s="39"/>
     </row>
     <row r="86" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="39"/>
-      <c r="B86" s="40"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="40"/>
-      <c r="F86" s="40"/>
-      <c r="G86" s="40"/>
+      <c r="A86" s="42"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="36"/>
+      <c r="G86" s="36"/>
       <c r="H86" s="16"/>
-      <c r="I86" s="40"/>
-      <c r="J86" s="40"/>
-      <c r="K86" s="42"/>
+      <c r="I86" s="36"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="38"/>
       <c r="L86" s="15" t="s">
         <v>8</v>
       </c>
@@ -4978,24 +4990,24 @@
       <c r="Q86" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="R86" s="43"/>
+      <c r="R86" s="40"/>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A87" s="38" t="s">
+      <c r="A87" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B87" s="38"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="38"/>
+      <c r="B87" s="33"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="33"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="33"/>
       <c r="G87" s="6">
         <v>5.1100000000000003</v>
       </c>
       <c r="H87" s="6"/>
-      <c r="I87" s="38"/>
-      <c r="J87" s="38"/>
-      <c r="K87" s="38"/>
+      <c r="I87" s="33"/>
+      <c r="J87" s="33"/>
+      <c r="K87" s="33"/>
       <c r="L87" s="6">
         <v>0</v>
       </c>
@@ -5005,25 +5017,25 @@
       <c r="N87" s="6">
         <v>0</v>
       </c>
-      <c r="O87" s="38"/>
-      <c r="P87" s="38"/>
-      <c r="Q87" s="38"/>
-      <c r="R87" s="38"/>
+      <c r="O87" s="33"/>
+      <c r="P87" s="33"/>
+      <c r="Q87" s="33"/>
+      <c r="R87" s="33"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A88" s="33"/>
-      <c r="B88" s="33"/>
-      <c r="C88" s="33"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="33"/>
-      <c r="F88" s="33"/>
+      <c r="A88" s="34"/>
+      <c r="B88" s="34"/>
+      <c r="C88" s="34"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="34"/>
+      <c r="F88" s="34"/>
       <c r="G88" s="3">
         <v>4.01</v>
       </c>
       <c r="H88" s="3"/>
-      <c r="I88" s="33"/>
-      <c r="J88" s="33"/>
-      <c r="K88" s="33"/>
+      <c r="I88" s="34"/>
+      <c r="J88" s="34"/>
+      <c r="K88" s="34"/>
       <c r="L88" s="3">
         <v>0</v>
       </c>
@@ -5033,25 +5045,25 @@
       <c r="N88" s="3">
         <v>0</v>
       </c>
-      <c r="O88" s="33"/>
-      <c r="P88" s="33"/>
-      <c r="Q88" s="33"/>
-      <c r="R88" s="33"/>
+      <c r="O88" s="34"/>
+      <c r="P88" s="34"/>
+      <c r="Q88" s="34"/>
+      <c r="R88" s="34"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A89" s="33"/>
-      <c r="B89" s="33"/>
-      <c r="C89" s="33"/>
-      <c r="D89" s="33"/>
-      <c r="E89" s="33"/>
-      <c r="F89" s="33"/>
+      <c r="A89" s="34"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="34"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="34"/>
+      <c r="F89" s="34"/>
       <c r="G89" s="3">
         <v>3.11</v>
       </c>
       <c r="H89" s="3"/>
-      <c r="I89" s="33"/>
-      <c r="J89" s="33"/>
-      <c r="K89" s="33"/>
+      <c r="I89" s="34"/>
+      <c r="J89" s="34"/>
+      <c r="K89" s="34"/>
       <c r="L89" s="3">
         <v>0</v>
       </c>
@@ -5061,25 +5073,25 @@
       <c r="N89" s="3">
         <v>0</v>
       </c>
-      <c r="O89" s="33"/>
-      <c r="P89" s="33"/>
-      <c r="Q89" s="33"/>
-      <c r="R89" s="33"/>
+      <c r="O89" s="34"/>
+      <c r="P89" s="34"/>
+      <c r="Q89" s="34"/>
+      <c r="R89" s="34"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A90" s="33"/>
-      <c r="B90" s="33"/>
-      <c r="C90" s="33"/>
-      <c r="D90" s="33"/>
-      <c r="E90" s="33"/>
-      <c r="F90" s="33"/>
+      <c r="A90" s="34"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="34"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
       <c r="G90" s="3">
         <v>1.98</v>
       </c>
       <c r="H90" s="3"/>
-      <c r="I90" s="33"/>
-      <c r="J90" s="33"/>
-      <c r="K90" s="33"/>
+      <c r="I90" s="34"/>
+      <c r="J90" s="34"/>
+      <c r="K90" s="34"/>
       <c r="L90" s="3">
         <v>18</v>
       </c>
@@ -5089,13 +5101,174 @@
       <c r="N90" s="3">
         <v>0</v>
       </c>
-      <c r="O90" s="33"/>
-      <c r="P90" s="33"/>
-      <c r="Q90" s="33"/>
-      <c r="R90" s="33"/>
+      <c r="O90" s="34"/>
+      <c r="P90" s="34"/>
+      <c r="Q90" s="34"/>
+      <c r="R90" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="185">
+    <mergeCell ref="J6:J10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J11:J15"/>
+    <mergeCell ref="K11:K15"/>
+    <mergeCell ref="K17:K21"/>
+    <mergeCell ref="R17:R21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="K22:K26"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="E17:E21"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="J27:J31"/>
+    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="R27:R31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="D42:D46"/>
+    <mergeCell ref="E42:E46"/>
+    <mergeCell ref="G32:G36"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="J32:J36"/>
+    <mergeCell ref="K32:K36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="F42:F46"/>
+    <mergeCell ref="G42:G46"/>
+    <mergeCell ref="I42:I46"/>
+    <mergeCell ref="J42:J46"/>
+    <mergeCell ref="K42:K46"/>
+    <mergeCell ref="R42:R46"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="J37:J41"/>
+    <mergeCell ref="K37:K41"/>
+    <mergeCell ref="R37:R41"/>
+    <mergeCell ref="Q47:Q51"/>
+    <mergeCell ref="R47:R51"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="D52:D56"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="F52:F56"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="I52:I56"/>
+    <mergeCell ref="G47:G51"/>
+    <mergeCell ref="I47:I51"/>
+    <mergeCell ref="J47:J51"/>
+    <mergeCell ref="K47:K51"/>
+    <mergeCell ref="O47:O51"/>
+    <mergeCell ref="P47:P51"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="C47:C51"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="E47:E51"/>
+    <mergeCell ref="F47:F51"/>
+    <mergeCell ref="J52:J56"/>
+    <mergeCell ref="K52:K56"/>
+    <mergeCell ref="R52:R56"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="E57:E61"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="I57:I61"/>
+    <mergeCell ref="J57:J61"/>
+    <mergeCell ref="K57:K61"/>
+    <mergeCell ref="R57:R61"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="C62:C66"/>
+    <mergeCell ref="D62:D66"/>
+    <mergeCell ref="E62:E66"/>
+    <mergeCell ref="F62:F66"/>
+    <mergeCell ref="R67:R71"/>
+    <mergeCell ref="A72:A76"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="C72:C76"/>
+    <mergeCell ref="D72:D76"/>
+    <mergeCell ref="E72:E76"/>
+    <mergeCell ref="G62:G66"/>
+    <mergeCell ref="I62:I66"/>
+    <mergeCell ref="J62:J66"/>
+    <mergeCell ref="K62:K66"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="C67:C71"/>
+    <mergeCell ref="D67:D71"/>
+    <mergeCell ref="E67:E71"/>
+    <mergeCell ref="F67:F71"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="C77:C81"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="E77:E81"/>
+    <mergeCell ref="G67:G71"/>
+    <mergeCell ref="I67:I71"/>
+    <mergeCell ref="J67:J71"/>
+    <mergeCell ref="K67:K71"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:D90"/>
+    <mergeCell ref="E87:E90"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="D82:D86"/>
+    <mergeCell ref="E82:E86"/>
     <mergeCell ref="F87:F90"/>
     <mergeCell ref="I87:I90"/>
     <mergeCell ref="J87:J90"/>
@@ -5120,167 +5293,6 @@
     <mergeCell ref="I72:I76"/>
     <mergeCell ref="J72:J76"/>
     <mergeCell ref="K72:K76"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="C87:C90"/>
-    <mergeCell ref="D87:D90"/>
-    <mergeCell ref="E87:E90"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="E82:E86"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="C77:C81"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="E77:E81"/>
-    <mergeCell ref="G67:G71"/>
-    <mergeCell ref="I67:I71"/>
-    <mergeCell ref="J67:J71"/>
-    <mergeCell ref="K67:K71"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="C62:C66"/>
-    <mergeCell ref="D62:D66"/>
-    <mergeCell ref="E62:E66"/>
-    <mergeCell ref="F62:F66"/>
-    <mergeCell ref="R67:R71"/>
-    <mergeCell ref="A72:A76"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="C72:C76"/>
-    <mergeCell ref="D72:D76"/>
-    <mergeCell ref="E72:E76"/>
-    <mergeCell ref="G62:G66"/>
-    <mergeCell ref="I62:I66"/>
-    <mergeCell ref="J62:J66"/>
-    <mergeCell ref="K62:K66"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="C67:C71"/>
-    <mergeCell ref="D67:D71"/>
-    <mergeCell ref="E67:E71"/>
-    <mergeCell ref="F67:F71"/>
-    <mergeCell ref="R52:R56"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="E57:E61"/>
-    <mergeCell ref="F57:F61"/>
-    <mergeCell ref="G57:G61"/>
-    <mergeCell ref="I57:I61"/>
-    <mergeCell ref="J57:J61"/>
-    <mergeCell ref="K57:K61"/>
-    <mergeCell ref="R57:R61"/>
-    <mergeCell ref="Q47:Q51"/>
-    <mergeCell ref="R47:R51"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="D52:D56"/>
-    <mergeCell ref="E52:E56"/>
-    <mergeCell ref="F52:F56"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="I52:I56"/>
-    <mergeCell ref="G47:G51"/>
-    <mergeCell ref="I47:I51"/>
-    <mergeCell ref="J47:J51"/>
-    <mergeCell ref="K47:K51"/>
-    <mergeCell ref="O47:O51"/>
-    <mergeCell ref="P47:P51"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="D47:D51"/>
-    <mergeCell ref="E47:E51"/>
-    <mergeCell ref="F47:F51"/>
-    <mergeCell ref="J52:J56"/>
-    <mergeCell ref="K52:K56"/>
-    <mergeCell ref="G42:G46"/>
-    <mergeCell ref="I42:I46"/>
-    <mergeCell ref="J42:J46"/>
-    <mergeCell ref="K42:K46"/>
-    <mergeCell ref="R42:R46"/>
-    <mergeCell ref="G37:G41"/>
-    <mergeCell ref="I37:I41"/>
-    <mergeCell ref="J37:J41"/>
-    <mergeCell ref="K37:K41"/>
-    <mergeCell ref="R37:R41"/>
-    <mergeCell ref="K27:K31"/>
-    <mergeCell ref="R27:R31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="E42:E46"/>
-    <mergeCell ref="G32:G36"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="J32:J36"/>
-    <mergeCell ref="K32:K36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="D37:D41"/>
-    <mergeCell ref="E37:E41"/>
-    <mergeCell ref="F37:F41"/>
-    <mergeCell ref="F42:F46"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="J27:J31"/>
-    <mergeCell ref="K17:K21"/>
-    <mergeCell ref="R17:R21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="G22:G26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="F17:F21"/>
-    <mergeCell ref="G17:G21"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="J6:J10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F11:F15"/>
-    <mergeCell ref="G11:G15"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="G6:G10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J11:J15"/>
-    <mergeCell ref="K11:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5293,34 +5305,37 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" customWidth="1"/>
     <col min="9" max="9" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>198</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>200</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="F1" t="s">
-        <v>166</v>
+        <v>202</v>
       </c>
       <c r="G1" t="s">
         <v>85</v>
@@ -5329,10 +5344,10 @@
         <v>86</v>
       </c>
       <c r="I1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -5393,7 +5408,7 @@
         <v>0.9</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J3" s="29">
         <v>32790</v>
@@ -5425,7 +5440,7 @@
         <v>0.9</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J4" s="29">
         <v>98500</v>
@@ -5457,7 +5472,7 @@
         <v>0.9</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J5" s="29">
         <v>97000</v>
@@ -5489,7 +5504,7 @@
         <v>0.8</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J6" s="29">
         <v>134500</v>
@@ -5553,7 +5568,7 @@
         <v>0.7</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J8" s="29">
         <v>81650</v>
@@ -5585,7 +5600,7 @@
         <v>0.6</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J9" s="29">
         <v>72000</v>
@@ -5617,7 +5632,7 @@
         <v>0.5</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J10" s="29">
         <v>16000</v>
@@ -5649,7 +5664,7 @@
         <v>0.4</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J11" s="29">
         <v>89500</v>
@@ -5681,7 +5696,7 @@
         <v>0.4</v>
       </c>
       <c r="I12" s="30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J12" s="29">
         <v>44910</v>
@@ -5777,7 +5792,7 @@
         <v>0.4</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J15" s="29">
         <v>15260</v>
@@ -5807,7 +5822,7 @@
       </c>
       <c r="H16" s="29"/>
       <c r="I16" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J16" s="29">
         <v>286300</v>
@@ -5856,8 +5871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6890CEF6-932C-244F-86BC-3348983EB407}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5881,45 +5896,45 @@
         <v>112</v>
       </c>
       <c r="B1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" t="s">
         <v>178</v>
       </c>
-      <c r="C1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>179</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>180</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K1" t="s">
         <v>181</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>182</v>
       </c>
-      <c r="I1" t="s">
-        <v>193</v>
-      </c>
-      <c r="J1" t="s">
-        <v>194</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>183</v>
-      </c>
-      <c r="L1" t="s">
-        <v>184</v>
-      </c>
-      <c r="M1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5960,7 +5975,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>-1</v>
@@ -6001,7 +6016,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -6042,7 +6057,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -6093,9 +6108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9B39B0-AFBE-1848-97F5-4C3DEB224DB7}">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6109,13 +6122,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6123,7 +6136,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -6137,7 +6150,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6151,7 +6164,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -6165,7 +6178,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -6179,7 +6192,7 @@
         <v>37</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -6193,7 +6206,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6207,7 +6220,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -6221,7 +6234,7 @@
         <v>52</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6235,7 +6248,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -6249,7 +6262,7 @@
         <v>57</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -6263,7 +6276,7 @@
         <v>60</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -6277,7 +6290,7 @@
         <v>62</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -6291,7 +6304,7 @@
         <v>66</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6305,7 +6318,7 @@
         <v>68</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -6319,7 +6332,7 @@
         <v>70</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -6333,7 +6346,7 @@
         <v>73</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -6347,7 +6360,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -6361,7 +6374,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -6375,7 +6388,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -6389,7 +6402,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -6403,7 +6416,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -6417,7 +6430,7 @@
         <v>41</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -6431,7 +6444,7 @@
         <v>47</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -6445,7 +6458,7 @@
         <v>52</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -6459,7 +6472,7 @@
         <v>57</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -6473,7 +6486,7 @@
         <v>60</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -6487,7 +6500,7 @@
         <v>62</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -6501,7 +6514,7 @@
         <v>66</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -6515,7 +6528,7 @@
         <v>68</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -6529,7 +6542,7 @@
         <v>70</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -6543,7 +6556,7 @@
         <v>73</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -6557,7 +6570,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -6571,7 +6584,7 @@
         <v>21</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -6585,7 +6598,7 @@
         <v>27</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -6599,7 +6612,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -6613,7 +6626,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -6627,7 +6640,7 @@
         <v>41</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -6641,7 +6654,7 @@
         <v>47</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -6655,7 +6668,7 @@
         <v>52</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -6669,7 +6682,7 @@
         <v>56</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -6683,7 +6696,7 @@
         <v>57</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -6697,7 +6710,7 @@
         <v>60</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -6711,7 +6724,7 @@
         <v>62</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -6725,7 +6738,7 @@
         <v>66</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -6739,7 +6752,7 @@
         <v>68</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -6753,7 +6766,7 @@
         <v>70</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -6767,7 +6780,7 @@
         <v>73</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -6781,7 +6794,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -6795,7 +6808,7 @@
         <v>21</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -6809,7 +6822,7 @@
         <v>27</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -6823,7 +6836,7 @@
         <v>32</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -6837,7 +6850,7 @@
         <v>37</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -6851,7 +6864,7 @@
         <v>41</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -6865,7 +6878,7 @@
         <v>47</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -6879,7 +6892,7 @@
         <v>52</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -6893,7 +6906,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -6907,7 +6920,7 @@
         <v>60</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -6921,7 +6934,7 @@
         <v>62</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -6935,7 +6948,7 @@
         <v>66</v>
       </c>
       <c r="B60" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -6949,7 +6962,7 @@
         <v>68</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -6963,7 +6976,7 @@
         <v>70</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -6977,7 +6990,7 @@
         <v>73</v>
       </c>
       <c r="B63" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -6991,7 +7004,7 @@
         <v>3</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -7005,7 +7018,7 @@
         <v>21</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -7019,7 +7032,7 @@
         <v>27</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -7033,7 +7046,7 @@
         <v>32</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -7047,7 +7060,7 @@
         <v>37</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -7061,7 +7074,7 @@
         <v>41</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -7075,7 +7088,7 @@
         <v>47</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -7089,7 +7102,7 @@
         <v>52</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -7103,7 +7116,7 @@
         <v>56</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -7117,7 +7130,7 @@
         <v>57</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -7131,7 +7144,7 @@
         <v>60</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -7145,7 +7158,7 @@
         <v>62</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -7159,7 +7172,7 @@
         <v>66</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -7173,7 +7186,7 @@
         <v>68</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -7187,7 +7200,7 @@
         <v>70</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -7201,7 +7214,7 @@
         <v>73</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -7215,7 +7228,7 @@
         <v>3</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -7229,7 +7242,7 @@
         <v>21</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -7243,7 +7256,7 @@
         <v>27</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -7257,7 +7270,7 @@
         <v>32</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -7271,7 +7284,7 @@
         <v>37</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -7285,7 +7298,7 @@
         <v>41</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -7299,7 +7312,7 @@
         <v>47</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -7313,7 +7326,7 @@
         <v>52</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -7327,7 +7340,7 @@
         <v>57</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -7341,7 +7354,7 @@
         <v>60</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -7355,7 +7368,7 @@
         <v>62</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -7369,7 +7382,7 @@
         <v>66</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -7383,7 +7396,7 @@
         <v>68</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -7397,7 +7410,7 @@
         <v>70</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -7411,7 +7424,7 @@
         <v>73</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -7425,7 +7438,7 @@
         <v>3</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -7439,7 +7452,7 @@
         <v>21</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -7453,7 +7466,7 @@
         <v>32</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -7467,7 +7480,7 @@
         <v>41</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -7481,7 +7494,7 @@
         <v>62</v>
       </c>
       <c r="B99" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -7495,7 +7508,7 @@
         <v>68</v>
       </c>
       <c r="B100" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C100">
         <v>0</v>

</xml_diff>

<commit_message>
Update notebook and data
</commit_message>
<xml_diff>
--- a/static/mock/AntiBio1.xlsx
+++ b/static/mock/AntiBio1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/PycharmProjects/ChemML/static/mock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2FA384-5CEB-B04E-AF06-7B62D8BA2668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DF3379-E838-A048-ADE1-182493F86803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{C97C895C-21C5-4ABD-B085-E1322DB1066B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="202">
   <si>
     <t>RE</t>
   </si>
@@ -674,9 +674,6 @@
     <t>Bacteria</t>
   </si>
   <si>
-    <t>Is_Salt</t>
-  </si>
-  <si>
     <t>Membrane pore diameter min</t>
   </si>
   <si>
@@ -701,19 +698,19 @@
     <t>REE</t>
   </si>
   <si>
-    <t xml:space="preserve">ionic_radii </t>
-  </si>
-  <si>
-    <t>electronegativity</t>
-  </si>
-  <si>
-    <t>crystal_structure_type</t>
-  </si>
-  <si>
-    <t>coordination_number_salt</t>
-  </si>
-  <si>
-    <t>coordination_number_solution</t>
+    <t>Is salt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ionic radii </t>
+  </si>
+  <si>
+    <t>Crystal structure type</t>
+  </si>
+  <si>
+    <t>Coordination number salt</t>
+  </si>
+  <si>
+    <t>Coordination number solution</t>
   </si>
 </sst>
 </file>
@@ -1131,37 +1128,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1493,11 +1490,11 @@
   <autoFilter ref="A1:J17" xr:uid="{2D3940D9-BD75-417D-B939-9D9F2B046451}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{6E3D35CA-3D70-45F1-9A50-18CBC54E9741}" name="REE" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{48794F88-A244-474D-A6B2-9FD63736CE7C}" name="ionic_radii " dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{DDE4413E-B094-4AFB-8138-A9932CA5D9D5}" name="electronegativity" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{CFF1D428-BCF1-46DF-ACB8-4EBDDD164153}" name="crystal_structure_type" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{0CA5AF80-08A7-4ED3-B39B-40669072521C}" name="coordination_number_salt" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{7FF2FE3D-DBC7-4F57-8794-C0C32F373CE2}" name="coordination_number_solution" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{48794F88-A244-474D-A6B2-9FD63736CE7C}" name="Ionic radii " dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{DDE4413E-B094-4AFB-8138-A9932CA5D9D5}" name="Electronegativity" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{CFF1D428-BCF1-46DF-ACB8-4EBDDD164153}" name="Crystal structure type" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{0CA5AF80-08A7-4ED3-B39B-40669072521C}" name="Coordination number salt" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{7FF2FE3D-DBC7-4F57-8794-C0C32F373CE2}" name="Coordination number solution" dataDxfId="14"/>
     <tableColumn id="7" xr3:uid="{3D5263EB-1B80-41C2-A1C6-35780FE385CD}" name="рН" dataDxfId="13"/>
     <tableColumn id="8" xr3:uid="{706A363A-7093-4406-B661-54FFDBA06FE1}" name="lgβ" dataDxfId="12"/>
     <tableColumn id="9" xr3:uid="{0FBAAE01-3DD2-4C00-AB7B-8504825C4F0D}" name="Electronic structure RE3+" dataDxfId="11"/>
@@ -1533,9 +1530,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9D9C3335-3503-2041-872A-E187CC19DAE4}" name="Table5" displayName="Table5" ref="A1:D100" totalsRowShown="0">
   <autoFilter ref="A1:D100" xr:uid="{9D9C3335-3503-2041-872A-E187CC19DAE4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858DE136-ED7D-8F41-B550-768E6C966C6F}" name="RE" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{858DE136-ED7D-8F41-B550-768E6C966C6F}" name="REE" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{77255B40-8DC1-3845-9724-E04D52CFAA47}" name="Bacteria" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{0C923B2D-D05B-9D4F-BD93-17B59A424B0D}" name="Is_Salt"/>
+    <tableColumn id="3" xr3:uid="{0C923B2D-D05B-9D4F-BD93-17B59A424B0D}" name="Is salt"/>
     <tableColumn id="4" xr3:uid="{55A8F227-AE1B-FF4C-8C62-9E53B05B48AF}" name="Stunting diameter"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1893,17 +1890,17 @@
       <c r="F1" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35" t="s">
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2065,35 +2062,35 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="33">
         <v>1.03</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="33">
         <v>2.4900000000000002</v>
       </c>
-      <c r="D6" s="34">
-        <v>1</v>
-      </c>
-      <c r="E6" s="34">
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+      <c r="E6" s="33">
         <v>11</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="33">
         <v>11</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="33">
         <v>4.4400000000000004</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="34">
+      <c r="I6" s="33">
         <v>0.8</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="34">
         <v>138000</v>
       </c>
       <c r="L6" s="13" t="s">
@@ -2119,17 +2116,17 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="37"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="34"/>
       <c r="L7" s="13" t="s">
         <v>6</v>
       </c>
@@ -2153,17 +2150,17 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="41"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="37"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="34"/>
       <c r="L8" s="13" t="s">
         <v>7</v>
       </c>
@@ -2187,17 +2184,17 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="37"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="34"/>
       <c r="L9" s="13" t="s">
         <v>8</v>
       </c>
@@ -2221,17 +2218,17 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="37"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="34"/>
       <c r="L10" s="25"/>
       <c r="M10" s="3" t="s">
         <v>13</v>
@@ -2253,35 +2250,35 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="33">
         <v>1.01</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="33">
         <v>2.61</v>
       </c>
-      <c r="D11" s="34">
-        <v>1</v>
-      </c>
-      <c r="E11" s="34">
+      <c r="D11" s="33">
+        <v>1</v>
+      </c>
+      <c r="E11" s="33">
         <v>11</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="33">
         <v>11</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="33">
         <v>4.2</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="34">
+      <c r="I11" s="33">
         <v>0.9</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="33">
         <v>601.42999999999995</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="34">
         <v>32790</v>
       </c>
       <c r="L11" s="13" t="s">
@@ -2307,17 +2304,17 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="41"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="37"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="34"/>
       <c r="L12" s="13" t="s">
         <v>16</v>
       </c>
@@ -2341,17 +2338,17 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="41"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="37"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="13" t="s">
         <v>17</v>
       </c>
@@ -2375,17 +2372,17 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="41"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="37"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="34"/>
       <c r="L14" s="13" t="s">
         <v>7</v>
       </c>
@@ -2409,17 +2406,17 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="41"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="37"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="34"/>
       <c r="L15" s="13" t="s">
         <v>8</v>
       </c>
@@ -2467,35 +2464,35 @@
       <c r="R16" s="14"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="33">
         <v>0.99</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="33">
         <v>2.2400000000000002</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="33">
         <v>2</v>
       </c>
-      <c r="E17" s="34">
-        <v>10</v>
-      </c>
-      <c r="F17" s="34">
-        <v>10</v>
-      </c>
-      <c r="G17" s="34">
+      <c r="E17" s="33">
+        <v>10</v>
+      </c>
+      <c r="F17" s="33">
+        <v>10</v>
+      </c>
+      <c r="G17" s="33">
         <v>4.51</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="34">
+      <c r="I17" s="33">
         <v>0.9</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="33">
         <v>602.42999999999995</v>
       </c>
-      <c r="K17" s="37">
+      <c r="K17" s="34">
         <v>98500</v>
       </c>
       <c r="L17" s="13" t="s">
@@ -2516,20 +2513,20 @@
       <c r="Q17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R17" s="39"/>
+      <c r="R17" s="36"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="41"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="37"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="34"/>
       <c r="L18" s="13" t="s">
         <v>16</v>
       </c>
@@ -2548,20 +2545,20 @@
       <c r="Q18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R18" s="39"/>
+      <c r="R18" s="36"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="41"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="37"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="34"/>
       <c r="L19" s="13" t="s">
         <v>17</v>
       </c>
@@ -2580,20 +2577,20 @@
       <c r="Q19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R19" s="39"/>
+      <c r="R19" s="36"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="41"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="37"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="34"/>
       <c r="L20" s="13" t="s">
         <v>7</v>
       </c>
@@ -2612,20 +2609,20 @@
       <c r="Q20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R20" s="39"/>
+      <c r="R20" s="36"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="41"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="37"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="34"/>
       <c r="L21" s="13" t="s">
         <v>8</v>
       </c>
@@ -2644,38 +2641,38 @@
       <c r="Q21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R21" s="39"/>
+      <c r="R21" s="36"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="34">
+      <c r="B22" s="33">
         <v>0.96</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="33">
         <v>1.9</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="33">
         <v>2</v>
       </c>
-      <c r="E22" s="34">
-        <v>10</v>
-      </c>
-      <c r="F22" s="34">
-        <v>10</v>
-      </c>
-      <c r="G22" s="34">
+      <c r="E22" s="33">
+        <v>10</v>
+      </c>
+      <c r="F22" s="33">
+        <v>10</v>
+      </c>
+      <c r="G22" s="33">
         <v>5.08</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="34">
+      <c r="I22" s="33">
         <v>0.9</v>
       </c>
-      <c r="J22" s="34">
+      <c r="J22" s="33">
         <v>602.43299999999999</v>
       </c>
-      <c r="K22" s="37">
+      <c r="K22" s="34">
         <v>97000</v>
       </c>
       <c r="L22" s="13" t="s">
@@ -2701,17 +2698,17 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="41"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="37"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="34"/>
       <c r="L23" s="13" t="s">
         <v>16</v>
       </c>
@@ -2735,17 +2732,17 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="41"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="37"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="34"/>
       <c r="L24" s="13" t="s">
         <v>17</v>
       </c>
@@ -2769,17 +2766,17 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="41"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="37"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="34"/>
       <c r="L25" s="13" t="s">
         <v>7</v>
       </c>
@@ -2803,17 +2800,17 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="41"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="37"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="34"/>
       <c r="L26" s="13" t="s">
         <v>8</v>
       </c>
@@ -2837,35 +2834,35 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="34">
+      <c r="B27" s="33">
         <v>0.95</v>
       </c>
-      <c r="C27" s="34">
+      <c r="C27" s="33">
         <v>1.81</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="33">
         <v>2</v>
       </c>
-      <c r="E27" s="34">
-        <v>10</v>
-      </c>
-      <c r="F27" s="34">
-        <v>10</v>
-      </c>
-      <c r="G27" s="34">
+      <c r="E27" s="33">
+        <v>10</v>
+      </c>
+      <c r="F27" s="33">
+        <v>10</v>
+      </c>
+      <c r="G27" s="33">
         <v>5.56</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="34">
+      <c r="I27" s="33">
         <v>0.8</v>
       </c>
-      <c r="J27" s="34">
+      <c r="J27" s="33">
         <v>602.43399999999997</v>
       </c>
-      <c r="K27" s="37">
+      <c r="K27" s="34">
         <v>134500</v>
       </c>
       <c r="L27" s="13" t="s">
@@ -2886,20 +2883,20 @@
       <c r="Q27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R27" s="39"/>
+      <c r="R27" s="36"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="41"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="37"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="34"/>
       <c r="L28" s="13" t="s">
         <v>16</v>
       </c>
@@ -2918,20 +2915,20 @@
       <c r="Q28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R28" s="39"/>
+      <c r="R28" s="36"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="41"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="37"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="34"/>
       <c r="L29" s="13" t="s">
         <v>17</v>
       </c>
@@ -2950,20 +2947,20 @@
       <c r="Q29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R29" s="39"/>
+      <c r="R29" s="36"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="37"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="34"/>
       <c r="L30" s="13" t="s">
         <v>7</v>
       </c>
@@ -2982,20 +2979,20 @@
       <c r="Q30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R30" s="39"/>
+      <c r="R30" s="36"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="41"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="37"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="34"/>
       <c r="L31" s="13" t="s">
         <v>8</v>
       </c>
@@ -3014,38 +3011,38 @@
       <c r="Q31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R31" s="39"/>
+      <c r="R31" s="36"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="34">
+      <c r="B32" s="33">
         <v>0.94</v>
       </c>
-      <c r="C32" s="34">
+      <c r="C32" s="33">
         <v>2.4</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="33">
         <v>2</v>
       </c>
-      <c r="E32" s="34">
-        <v>10</v>
-      </c>
-      <c r="F32" s="34">
-        <v>10</v>
-      </c>
-      <c r="G32" s="34">
+      <c r="E32" s="33">
+        <v>10</v>
+      </c>
+      <c r="F32" s="33">
+        <v>10</v>
+      </c>
+      <c r="G32" s="33">
         <v>4.51</v>
       </c>
       <c r="H32" s="3"/>
-      <c r="I32" s="34">
+      <c r="I32" s="33">
         <v>0.8</v>
       </c>
-      <c r="J32" s="34" t="s">
+      <c r="J32" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="K32" s="37">
+      <c r="K32" s="34">
         <v>78450</v>
       </c>
       <c r="L32" s="13" t="s">
@@ -3071,17 +3068,17 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" s="41"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="37"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="34"/>
       <c r="L33" s="13" t="s">
         <v>16</v>
       </c>
@@ -3105,17 +3102,17 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A34" s="41"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="37"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="34"/>
       <c r="L34" s="13" t="s">
         <v>17</v>
       </c>
@@ -3139,17 +3136,17 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A35" s="41"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="37"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="34"/>
       <c r="L35" s="13" t="s">
         <v>7</v>
       </c>
@@ -3173,17 +3170,17 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" s="41"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="37"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="34"/>
       <c r="L36" s="13" t="s">
         <v>8</v>
       </c>
@@ -3207,35 +3204,35 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="34">
+      <c r="B37" s="33">
         <v>0.92</v>
       </c>
-      <c r="C37" s="34">
+      <c r="C37" s="33">
         <v>2.29</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D37" s="33">
         <v>2</v>
       </c>
-      <c r="E37" s="34">
-        <v>10</v>
-      </c>
-      <c r="F37" s="34">
-        <v>10</v>
-      </c>
-      <c r="G37" s="34">
+      <c r="E37" s="33">
+        <v>10</v>
+      </c>
+      <c r="F37" s="33">
+        <v>10</v>
+      </c>
+      <c r="G37" s="33">
         <v>1.87</v>
       </c>
       <c r="H37" s="3"/>
-      <c r="I37" s="34">
+      <c r="I37" s="33">
         <v>0.7</v>
       </c>
-      <c r="J37" s="34">
+      <c r="J37" s="33">
         <v>602.43600000000004</v>
       </c>
-      <c r="K37" s="37">
+      <c r="K37" s="34">
         <v>81650</v>
       </c>
       <c r="L37" s="13" t="s">
@@ -3256,20 +3253,20 @@
       <c r="Q37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R37" s="39"/>
+      <c r="R37" s="36"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" s="41"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="37"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="34"/>
       <c r="L38" s="13" t="s">
         <v>16</v>
       </c>
@@ -3288,20 +3285,20 @@
       <c r="Q38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R38" s="39"/>
+      <c r="R38" s="36"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="41"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="37"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="34"/>
       <c r="L39" s="13" t="s">
         <v>17</v>
       </c>
@@ -3320,20 +3317,20 @@
       <c r="Q39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R39" s="39"/>
+      <c r="R39" s="36"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" s="41"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="37"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="34"/>
       <c r="L40" s="13" t="s">
         <v>7</v>
       </c>
@@ -3352,20 +3349,20 @@
       <c r="Q40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R40" s="39"/>
+      <c r="R40" s="36"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A41" s="41"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
+      <c r="A41" s="35"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="34"/>
-      <c r="K41" s="37"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="34"/>
       <c r="L41" s="13" t="s">
         <v>8</v>
       </c>
@@ -3384,38 +3381,38 @@
       <c r="Q41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R41" s="39"/>
+      <c r="R41" s="36"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="34">
+      <c r="B42" s="33">
         <v>0.91</v>
       </c>
-      <c r="C42" s="34">
+      <c r="C42" s="33">
         <v>2.0699999999999998</v>
       </c>
-      <c r="D42" s="34">
+      <c r="D42" s="33">
         <v>3</v>
       </c>
-      <c r="E42" s="34">
-        <v>10</v>
-      </c>
-      <c r="F42" s="34">
-        <v>10</v>
-      </c>
-      <c r="G42" s="34">
+      <c r="E42" s="33">
+        <v>10</v>
+      </c>
+      <c r="F42" s="33">
+        <v>10</v>
+      </c>
+      <c r="G42" s="33">
         <v>5.78</v>
       </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="34">
+      <c r="I42" s="33">
         <v>0.6</v>
       </c>
-      <c r="J42" s="34">
+      <c r="J42" s="33">
         <v>602.43700000000001</v>
       </c>
-      <c r="K42" s="37">
+      <c r="K42" s="34">
         <v>72000</v>
       </c>
       <c r="L42" s="13" t="s">
@@ -3436,20 +3433,20 @@
       <c r="Q42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R42" s="39"/>
+      <c r="R42" s="36"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" s="41"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
-      <c r="K43" s="37"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="34"/>
       <c r="L43" s="13" t="s">
         <v>16</v>
       </c>
@@ -3468,20 +3465,20 @@
       <c r="Q43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R43" s="39"/>
+      <c r="R43" s="36"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A44" s="41"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
-      <c r="K44" s="37"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="34"/>
       <c r="L44" s="13" t="s">
         <v>17</v>
       </c>
@@ -3500,20 +3497,20 @@
       <c r="Q44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R44" s="39"/>
+      <c r="R44" s="36"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="41"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
-      <c r="K45" s="37"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="34"/>
       <c r="L45" s="13" t="s">
         <v>7</v>
       </c>
@@ -3532,20 +3529,20 @@
       <c r="Q45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R45" s="39"/>
+      <c r="R45" s="36"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="41"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="37"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="34"/>
       <c r="L46" s="13" t="s">
         <v>8</v>
       </c>
@@ -3564,38 +3561,38 @@
       <c r="Q46" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R46" s="39"/>
+      <c r="R46" s="36"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="34">
+      <c r="B47" s="33">
         <v>0.9</v>
       </c>
-      <c r="C47" s="34">
+      <c r="C47" s="33">
         <v>2.12</v>
       </c>
-      <c r="D47" s="34">
+      <c r="D47" s="33">
         <v>3</v>
       </c>
-      <c r="E47" s="34">
+      <c r="E47" s="33">
         <v>9</v>
       </c>
-      <c r="F47" s="34">
+      <c r="F47" s="33">
         <v>9</v>
       </c>
-      <c r="G47" s="34">
+      <c r="G47" s="33">
         <v>5.96</v>
       </c>
       <c r="H47" s="3"/>
-      <c r="I47" s="34">
+      <c r="I47" s="33">
         <v>0.5</v>
       </c>
-      <c r="J47" s="34">
+      <c r="J47" s="33">
         <v>602.43799999999999</v>
       </c>
-      <c r="K47" s="37">
+      <c r="K47" s="34">
         <v>16000</v>
       </c>
       <c r="L47" s="13" t="s">
@@ -3607,23 +3604,23 @@
       <c r="N47" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="O47" s="43"/>
-      <c r="P47" s="34"/>
-      <c r="Q47" s="34"/>
-      <c r="R47" s="39"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="36"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A48" s="41"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="37"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="34"/>
       <c r="L48" s="13" t="s">
         <v>16</v>
       </c>
@@ -3633,23 +3630,23 @@
       <c r="N48" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="O48" s="43"/>
-      <c r="P48" s="34"/>
-      <c r="Q48" s="34"/>
-      <c r="R48" s="39"/>
+      <c r="O48" s="37"/>
+      <c r="P48" s="33"/>
+      <c r="Q48" s="33"/>
+      <c r="R48" s="36"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" s="41"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="37"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="34"/>
       <c r="L49" s="13" t="s">
         <v>17</v>
       </c>
@@ -3659,23 +3656,23 @@
       <c r="N49" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="O49" s="43"/>
-      <c r="P49" s="34"/>
-      <c r="Q49" s="34"/>
-      <c r="R49" s="39"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="36"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A50" s="41"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="37"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="34"/>
       <c r="L50" s="13" t="s">
         <v>7</v>
       </c>
@@ -3685,23 +3682,23 @@
       <c r="N50" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="O50" s="43"/>
-      <c r="P50" s="34"/>
-      <c r="Q50" s="34"/>
-      <c r="R50" s="39"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="33"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="36"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A51" s="41"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
+      <c r="A51" s="35"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="37"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="34"/>
       <c r="L51" s="13" t="s">
         <v>8</v>
       </c>
@@ -3711,41 +3708,41 @@
       <c r="N51" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O51" s="43"/>
-      <c r="P51" s="34"/>
-      <c r="Q51" s="34"/>
-      <c r="R51" s="39"/>
+      <c r="O51" s="37"/>
+      <c r="P51" s="33"/>
+      <c r="Q51" s="33"/>
+      <c r="R51" s="36"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A52" s="41" t="s">
+      <c r="A52" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="34">
+      <c r="B52" s="33">
         <v>0.89</v>
       </c>
-      <c r="C52" s="34">
+      <c r="C52" s="33">
         <v>2.02</v>
       </c>
-      <c r="D52" s="34">
+      <c r="D52" s="33">
         <v>4</v>
       </c>
-      <c r="E52" s="34">
+      <c r="E52" s="33">
         <v>9</v>
       </c>
-      <c r="F52" s="34">
+      <c r="F52" s="33">
         <v>9</v>
       </c>
-      <c r="G52" s="34">
+      <c r="G52" s="33">
         <v>5.16</v>
       </c>
       <c r="H52" s="3"/>
-      <c r="I52" s="34">
+      <c r="I52" s="33">
         <v>0.4</v>
       </c>
-      <c r="J52" s="34">
+      <c r="J52" s="33">
         <v>602.43899999999996</v>
       </c>
-      <c r="K52" s="37">
+      <c r="K52" s="34">
         <v>89500</v>
       </c>
       <c r="L52" s="13" t="s">
@@ -3766,20 +3763,20 @@
       <c r="Q52" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R52" s="39"/>
+      <c r="R52" s="36"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A53" s="41"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
+      <c r="A53" s="35"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="34"/>
-      <c r="K53" s="37"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="34"/>
       <c r="L53" s="13" t="s">
         <v>16</v>
       </c>
@@ -3798,20 +3795,20 @@
       <c r="Q53" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R53" s="39"/>
+      <c r="R53" s="36"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="41"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
+      <c r="A54" s="35"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="37"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="34"/>
       <c r="L54" s="13" t="s">
         <v>17</v>
       </c>
@@ -3830,20 +3827,20 @@
       <c r="Q54" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R54" s="39"/>
+      <c r="R54" s="36"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="41"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="34"/>
+      <c r="A55" s="35"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="34"/>
-      <c r="K55" s="37"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="34"/>
       <c r="L55" s="13" t="s">
         <v>7</v>
       </c>
@@ -3862,20 +3859,20 @@
       <c r="Q55" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R55" s="39"/>
+      <c r="R55" s="36"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="41"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
+      <c r="A56" s="35"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="34"/>
-      <c r="K56" s="37"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="34"/>
       <c r="L56" s="13" t="s">
         <v>8</v>
       </c>
@@ -3894,38 +3891,38 @@
       <c r="Q56" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R56" s="39"/>
+      <c r="R56" s="36"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="34">
+      <c r="B57" s="33">
         <v>0.88</v>
       </c>
-      <c r="C57" s="34">
+      <c r="C57" s="33">
         <v>2.0299999999999998</v>
       </c>
-      <c r="D57" s="34">
+      <c r="D57" s="33">
         <v>4</v>
       </c>
-      <c r="E57" s="34">
+      <c r="E57" s="33">
         <v>9</v>
       </c>
-      <c r="F57" s="34">
+      <c r="F57" s="33">
         <v>9</v>
       </c>
-      <c r="G57" s="34">
+      <c r="G57" s="33">
         <v>5.54</v>
       </c>
       <c r="H57" s="3"/>
-      <c r="I57" s="34">
+      <c r="I57" s="33">
         <v>0.4</v>
       </c>
-      <c r="J57" s="34">
+      <c r="J57" s="33">
         <v>602.43100000000004</v>
       </c>
-      <c r="K57" s="37">
+      <c r="K57" s="34">
         <v>44910</v>
       </c>
       <c r="L57" s="13" t="s">
@@ -3946,20 +3943,20 @@
       <c r="Q57" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R57" s="39"/>
+      <c r="R57" s="36"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="41"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
+      <c r="A58" s="35"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
-      <c r="K58" s="37"/>
+      <c r="I58" s="33"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="34"/>
       <c r="L58" s="13" t="s">
         <v>16</v>
       </c>
@@ -3978,20 +3975,20 @@
       <c r="Q58" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R58" s="39"/>
+      <c r="R58" s="36"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A59" s="41"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
-      <c r="K59" s="37"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="34"/>
       <c r="L59" s="13" t="s">
         <v>17</v>
       </c>
@@ -4010,20 +4007,20 @@
       <c r="Q59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R59" s="39"/>
+      <c r="R59" s="36"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="41"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
+      <c r="A60" s="35"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="37"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="34"/>
       <c r="L60" s="13" t="s">
         <v>7</v>
       </c>
@@ -4042,20 +4039,20 @@
       <c r="Q60" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R60" s="39"/>
+      <c r="R60" s="36"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="41"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34"/>
+      <c r="A61" s="35"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="33"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="37"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="34"/>
       <c r="L61" s="13" t="s">
         <v>8</v>
       </c>
@@ -4074,38 +4071,38 @@
       <c r="Q61" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R61" s="39"/>
+      <c r="R61" s="36"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A62" s="41" t="s">
+      <c r="A62" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="34">
+      <c r="B62" s="33">
         <v>0.87</v>
       </c>
-      <c r="C62" s="34">
+      <c r="C62" s="33">
         <v>1.78</v>
       </c>
-      <c r="D62" s="34">
+      <c r="D62" s="33">
         <v>5</v>
       </c>
-      <c r="E62" s="34">
+      <c r="E62" s="33">
         <v>9</v>
       </c>
-      <c r="F62" s="34">
+      <c r="F62" s="33">
         <v>9</v>
       </c>
-      <c r="G62" s="34">
+      <c r="G62" s="33">
         <v>5.74</v>
       </c>
       <c r="H62" s="3"/>
-      <c r="I62" s="34">
+      <c r="I62" s="33">
         <v>0.4</v>
       </c>
-      <c r="J62" s="34" t="s">
+      <c r="J62" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="K62" s="37">
+      <c r="K62" s="34">
         <v>84040</v>
       </c>
       <c r="L62" s="13" t="s">
@@ -4131,17 +4128,17 @@
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="41"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
+      <c r="A63" s="35"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="33"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="37"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="33"/>
+      <c r="K63" s="34"/>
       <c r="L63" s="13" t="s">
         <v>16</v>
       </c>
@@ -4165,17 +4162,17 @@
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="41"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="34"/>
+      <c r="A64" s="35"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="34"/>
-      <c r="J64" s="34"/>
-      <c r="K64" s="37"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="34"/>
       <c r="L64" s="13" t="s">
         <v>17</v>
       </c>
@@ -4199,17 +4196,17 @@
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A65" s="41"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
+      <c r="A65" s="35"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="34"/>
-      <c r="J65" s="34"/>
-      <c r="K65" s="37"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="34"/>
       <c r="L65" s="13" t="s">
         <v>7</v>
       </c>
@@ -4233,17 +4230,17 @@
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A66" s="41"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="34"/>
+      <c r="A66" s="35"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="34"/>
-      <c r="J66" s="34"/>
-      <c r="K66" s="37"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33"/>
+      <c r="K66" s="34"/>
       <c r="L66" s="13" t="s">
         <v>8</v>
       </c>
@@ -4267,35 +4264,35 @@
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="34">
+      <c r="B67" s="33">
         <v>0.86</v>
       </c>
-      <c r="C67" s="34">
+      <c r="C67" s="33">
         <v>2.68</v>
       </c>
-      <c r="D67" s="34">
+      <c r="D67" s="33">
         <v>7</v>
       </c>
-      <c r="E67" s="34">
+      <c r="E67" s="33">
         <v>9</v>
       </c>
-      <c r="F67" s="34">
+      <c r="F67" s="33">
         <v>9</v>
       </c>
-      <c r="G67" s="34">
+      <c r="G67" s="33">
         <v>5.5</v>
       </c>
       <c r="H67" s="3"/>
-      <c r="I67" s="34">
+      <c r="I67" s="33">
         <v>0.6</v>
       </c>
-      <c r="J67" s="34" t="s">
+      <c r="J67" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K67" s="37">
+      <c r="K67" s="34">
         <v>252000</v>
       </c>
       <c r="L67" s="13" t="s">
@@ -4316,20 +4313,20 @@
       <c r="Q67" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="R67" s="39"/>
+      <c r="R67" s="36"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A68" s="41"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="34"/>
+      <c r="A68" s="35"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="33"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="34"/>
-      <c r="J68" s="34"/>
-      <c r="K68" s="37"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="33"/>
+      <c r="K68" s="34"/>
       <c r="L68" s="13" t="s">
         <v>16</v>
       </c>
@@ -4348,20 +4345,20 @@
       <c r="Q68" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R68" s="39"/>
+      <c r="R68" s="36"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A69" s="41"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="34"/>
+      <c r="A69" s="35"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="34"/>
-      <c r="J69" s="34"/>
-      <c r="K69" s="37"/>
+      <c r="I69" s="33"/>
+      <c r="J69" s="33"/>
+      <c r="K69" s="34"/>
       <c r="L69" s="13" t="s">
         <v>17</v>
       </c>
@@ -4380,20 +4377,20 @@
       <c r="Q69" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R69" s="39"/>
+      <c r="R69" s="36"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A70" s="41"/>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="34"/>
+      <c r="A70" s="35"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="33"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="34"/>
-      <c r="J70" s="34"/>
-      <c r="K70" s="37"/>
+      <c r="I70" s="33"/>
+      <c r="J70" s="33"/>
+      <c r="K70" s="34"/>
       <c r="L70" s="13" t="s">
         <v>7</v>
       </c>
@@ -4412,20 +4409,20 @@
       <c r="Q70" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R70" s="39"/>
+      <c r="R70" s="36"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A71" s="41"/>
-      <c r="B71" s="34"/>
-      <c r="C71" s="34"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34"/>
+      <c r="A71" s="35"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="33"/>
       <c r="H71" s="3"/>
-      <c r="I71" s="34"/>
-      <c r="J71" s="34"/>
-      <c r="K71" s="37"/>
+      <c r="I71" s="33"/>
+      <c r="J71" s="33"/>
+      <c r="K71" s="34"/>
       <c r="L71" s="13" t="s">
         <v>8</v>
       </c>
@@ -4444,38 +4441,38 @@
       <c r="Q71" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R71" s="39"/>
+      <c r="R71" s="36"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="34">
+      <c r="B72" s="33">
         <v>0.9</v>
       </c>
-      <c r="C72" s="34">
+      <c r="C72" s="33">
         <v>2.52</v>
       </c>
-      <c r="D72" s="34">
+      <c r="D72" s="33">
         <v>2</v>
       </c>
-      <c r="E72" s="34">
-        <v>10</v>
-      </c>
-      <c r="F72" s="34">
-        <v>10</v>
-      </c>
-      <c r="G72" s="34">
+      <c r="E72" s="33">
+        <v>10</v>
+      </c>
+      <c r="F72" s="33">
+        <v>10</v>
+      </c>
+      <c r="G72" s="33">
         <v>5.92</v>
       </c>
       <c r="H72" s="3"/>
-      <c r="I72" s="34">
+      <c r="I72" s="33">
         <v>0.4</v>
       </c>
-      <c r="J72" s="34">
+      <c r="J72" s="33">
         <v>500.42</v>
       </c>
-      <c r="K72" s="37">
+      <c r="K72" s="34">
         <v>15260</v>
       </c>
       <c r="L72" s="13" t="s">
@@ -4501,17 +4498,17 @@
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A73" s="41"/>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
-      <c r="F73" s="34"/>
-      <c r="G73" s="34"/>
+      <c r="A73" s="35"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="33"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="34"/>
-      <c r="J73" s="34"/>
-      <c r="K73" s="37"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+      <c r="K73" s="34"/>
       <c r="L73" s="13" t="s">
         <v>16</v>
       </c>
@@ -4535,17 +4532,17 @@
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A74" s="41"/>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="34"/>
+      <c r="A74" s="35"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="33"/>
+      <c r="E74" s="33"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="33"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="34"/>
-      <c r="J74" s="34"/>
-      <c r="K74" s="37"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="33"/>
+      <c r="K74" s="34"/>
       <c r="L74" s="13" t="s">
         <v>17</v>
       </c>
@@ -4569,17 +4566,17 @@
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A75" s="41"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="34"/>
+      <c r="A75" s="35"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="33"/>
+      <c r="E75" s="33"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="33"/>
       <c r="H75" s="3"/>
-      <c r="I75" s="34"/>
-      <c r="J75" s="34"/>
-      <c r="K75" s="37"/>
+      <c r="I75" s="33"/>
+      <c r="J75" s="33"/>
+      <c r="K75" s="34"/>
       <c r="L75" s="13" t="s">
         <v>7</v>
       </c>
@@ -4603,17 +4600,17 @@
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A76" s="41"/>
-      <c r="B76" s="34"/>
-      <c r="C76" s="34"/>
-      <c r="D76" s="34"/>
-      <c r="E76" s="34"/>
-      <c r="F76" s="34"/>
-      <c r="G76" s="34"/>
+      <c r="A76" s="35"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="34"/>
-      <c r="J76" s="34"/>
-      <c r="K76" s="37"/>
+      <c r="I76" s="33"/>
+      <c r="J76" s="33"/>
+      <c r="K76" s="34"/>
       <c r="L76" s="13" t="s">
         <v>8</v>
       </c>
@@ -4637,33 +4634,33 @@
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B77" s="34">
+      <c r="B77" s="33">
         <v>0.75</v>
       </c>
-      <c r="C77" s="34">
+      <c r="C77" s="33">
         <v>2.35</v>
       </c>
-      <c r="D77" s="34">
+      <c r="D77" s="33">
         <v>6</v>
       </c>
-      <c r="E77" s="34">
+      <c r="E77" s="33">
         <v>6</v>
       </c>
-      <c r="F77" s="34">
+      <c r="F77" s="33">
         <v>6</v>
       </c>
-      <c r="G77" s="34">
+      <c r="G77" s="33">
         <v>2.0299999999999998</v>
       </c>
       <c r="H77" s="3"/>
-      <c r="I77" s="34"/>
-      <c r="J77" s="34">
+      <c r="I77" s="33"/>
+      <c r="J77" s="33">
         <v>400.32</v>
       </c>
-      <c r="K77" s="37">
+      <c r="K77" s="34">
         <v>286300</v>
       </c>
       <c r="L77" s="13" t="s">
@@ -4684,20 +4681,20 @@
       <c r="Q77" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R77" s="39"/>
+      <c r="R77" s="36"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A78" s="41"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="34"/>
-      <c r="D78" s="34"/>
-      <c r="E78" s="34"/>
-      <c r="F78" s="34"/>
-      <c r="G78" s="34"/>
+      <c r="A78" s="35"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="33"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="33"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="34"/>
-      <c r="J78" s="34"/>
-      <c r="K78" s="37"/>
+      <c r="I78" s="33"/>
+      <c r="J78" s="33"/>
+      <c r="K78" s="34"/>
       <c r="L78" s="13" t="s">
         <v>16</v>
       </c>
@@ -4716,20 +4713,20 @@
       <c r="Q78" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R78" s="39"/>
+      <c r="R78" s="36"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A79" s="41"/>
-      <c r="B79" s="34"/>
-      <c r="C79" s="34"/>
-      <c r="D79" s="34"/>
-      <c r="E79" s="34"/>
-      <c r="F79" s="34"/>
-      <c r="G79" s="34"/>
+      <c r="A79" s="35"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="33"/>
+      <c r="D79" s="33"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="33"/>
       <c r="H79" s="3"/>
-      <c r="I79" s="34"/>
-      <c r="J79" s="34"/>
-      <c r="K79" s="37"/>
+      <c r="I79" s="33"/>
+      <c r="J79" s="33"/>
+      <c r="K79" s="34"/>
       <c r="L79" s="13" t="s">
         <v>17</v>
       </c>
@@ -4748,20 +4745,20 @@
       <c r="Q79" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R79" s="39"/>
+      <c r="R79" s="36"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A80" s="41"/>
-      <c r="B80" s="34"/>
-      <c r="C80" s="34"/>
-      <c r="D80" s="34"/>
-      <c r="E80" s="34"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="34"/>
+      <c r="A80" s="35"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
       <c r="H80" s="3"/>
-      <c r="I80" s="34"/>
-      <c r="J80" s="34"/>
-      <c r="K80" s="37"/>
+      <c r="I80" s="33"/>
+      <c r="J80" s="33"/>
+      <c r="K80" s="34"/>
       <c r="L80" s="13" t="s">
         <v>7</v>
       </c>
@@ -4780,20 +4777,20 @@
       <c r="Q80" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R80" s="39"/>
+      <c r="R80" s="36"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A81" s="41"/>
-      <c r="B81" s="34"/>
-      <c r="C81" s="34"/>
-      <c r="D81" s="34"/>
-      <c r="E81" s="34"/>
-      <c r="F81" s="34"/>
-      <c r="G81" s="34"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="33"/>
+      <c r="E81" s="33"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="33"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="34"/>
-      <c r="J81" s="34"/>
-      <c r="K81" s="37"/>
+      <c r="I81" s="33"/>
+      <c r="J81" s="33"/>
+      <c r="K81" s="34"/>
       <c r="L81" s="13" t="s">
         <v>8</v>
       </c>
@@ -4812,36 +4809,36 @@
       <c r="Q81" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R81" s="39"/>
+      <c r="R81" s="36"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A82" s="41" t="s">
+      <c r="A82" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B82" s="34">
-        <v>1</v>
-      </c>
-      <c r="C82" s="34">
+      <c r="B82" s="33">
+        <v>1</v>
+      </c>
+      <c r="C82" s="33">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D82" s="34">
+      <c r="D82" s="33">
         <v>7</v>
       </c>
-      <c r="E82" s="34">
+      <c r="E82" s="33">
         <v>6</v>
       </c>
-      <c r="F82" s="34">
+      <c r="F82" s="33">
         <v>6</v>
       </c>
-      <c r="G82" s="34">
+      <c r="G82" s="33">
         <v>5.63</v>
       </c>
       <c r="H82" s="3"/>
-      <c r="I82" s="34"/>
-      <c r="J82" s="34">
+      <c r="I82" s="33"/>
+      <c r="J82" s="33">
         <v>400</v>
       </c>
-      <c r="K82" s="37" t="s">
+      <c r="K82" s="34" t="s">
         <v>74</v>
       </c>
       <c r="L82" s="13" t="s">
@@ -4862,20 +4859,20 @@
       <c r="Q82" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R82" s="39"/>
+      <c r="R82" s="36"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A83" s="41"/>
-      <c r="B83" s="34"/>
-      <c r="C83" s="34"/>
-      <c r="D83" s="34"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="34"/>
+      <c r="A83" s="35"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="34"/>
-      <c r="J83" s="34"/>
-      <c r="K83" s="37"/>
+      <c r="I83" s="33"/>
+      <c r="J83" s="33"/>
+      <c r="K83" s="34"/>
       <c r="L83" s="13" t="s">
         <v>16</v>
       </c>
@@ -4894,20 +4891,20 @@
       <c r="Q83" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R83" s="39"/>
+      <c r="R83" s="36"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A84" s="41"/>
-      <c r="B84" s="34"/>
-      <c r="C84" s="34"/>
-      <c r="D84" s="34"/>
-      <c r="E84" s="34"/>
-      <c r="F84" s="34"/>
-      <c r="G84" s="34"/>
+      <c r="A84" s="35"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="33"/>
+      <c r="F84" s="33"/>
+      <c r="G84" s="33"/>
       <c r="H84" s="3"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="34"/>
-      <c r="K84" s="37"/>
+      <c r="I84" s="33"/>
+      <c r="J84" s="33"/>
+      <c r="K84" s="34"/>
       <c r="L84" s="13" t="s">
         <v>17</v>
       </c>
@@ -4926,20 +4923,20 @@
       <c r="Q84" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R84" s="39"/>
+      <c r="R84" s="36"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A85" s="41"/>
-      <c r="B85" s="34"/>
-      <c r="C85" s="34"/>
-      <c r="D85" s="34"/>
-      <c r="E85" s="34"/>
-      <c r="F85" s="34"/>
-      <c r="G85" s="34"/>
+      <c r="A85" s="35"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="33"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="33"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="34"/>
-      <c r="J85" s="34"/>
-      <c r="K85" s="37"/>
+      <c r="I85" s="33"/>
+      <c r="J85" s="33"/>
+      <c r="K85" s="34"/>
       <c r="L85" s="13" t="s">
         <v>7</v>
       </c>
@@ -4958,20 +4955,20 @@
       <c r="Q85" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R85" s="39"/>
+      <c r="R85" s="36"/>
     </row>
     <row r="86" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="42"/>
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="36"/>
+      <c r="A86" s="39"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="40"/>
+      <c r="F86" s="40"/>
+      <c r="G86" s="40"/>
       <c r="H86" s="16"/>
-      <c r="I86" s="36"/>
-      <c r="J86" s="36"/>
-      <c r="K86" s="38"/>
+      <c r="I86" s="40"/>
+      <c r="J86" s="40"/>
+      <c r="K86" s="42"/>
       <c r="L86" s="15" t="s">
         <v>8</v>
       </c>
@@ -4990,24 +4987,24 @@
       <c r="Q86" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="R86" s="40"/>
+      <c r="R86" s="43"/>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A87" s="33" t="s">
+      <c r="A87" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B87" s="33"/>
-      <c r="C87" s="33"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="33"/>
-      <c r="F87" s="33"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38"/>
       <c r="G87" s="6">
         <v>5.1100000000000003</v>
       </c>
       <c r="H87" s="6"/>
-      <c r="I87" s="33"/>
-      <c r="J87" s="33"/>
-      <c r="K87" s="33"/>
+      <c r="I87" s="38"/>
+      <c r="J87" s="38"/>
+      <c r="K87" s="38"/>
       <c r="L87" s="6">
         <v>0</v>
       </c>
@@ -5017,25 +5014,25 @@
       <c r="N87" s="6">
         <v>0</v>
       </c>
-      <c r="O87" s="33"/>
-      <c r="P87" s="33"/>
-      <c r="Q87" s="33"/>
-      <c r="R87" s="33"/>
+      <c r="O87" s="38"/>
+      <c r="P87" s="38"/>
+      <c r="Q87" s="38"/>
+      <c r="R87" s="38"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A88" s="34"/>
-      <c r="B88" s="34"/>
-      <c r="C88" s="34"/>
-      <c r="D88" s="34"/>
-      <c r="E88" s="34"/>
-      <c r="F88" s="34"/>
+      <c r="A88" s="33"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
       <c r="G88" s="3">
         <v>4.01</v>
       </c>
       <c r="H88" s="3"/>
-      <c r="I88" s="34"/>
-      <c r="J88" s="34"/>
-      <c r="K88" s="34"/>
+      <c r="I88" s="33"/>
+      <c r="J88" s="33"/>
+      <c r="K88" s="33"/>
       <c r="L88" s="3">
         <v>0</v>
       </c>
@@ -5045,25 +5042,25 @@
       <c r="N88" s="3">
         <v>0</v>
       </c>
-      <c r="O88" s="34"/>
-      <c r="P88" s="34"/>
-      <c r="Q88" s="34"/>
-      <c r="R88" s="34"/>
+      <c r="O88" s="33"/>
+      <c r="P88" s="33"/>
+      <c r="Q88" s="33"/>
+      <c r="R88" s="33"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A89" s="34"/>
-      <c r="B89" s="34"/>
-      <c r="C89" s="34"/>
-      <c r="D89" s="34"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="34"/>
+      <c r="A89" s="33"/>
+      <c r="B89" s="33"/>
+      <c r="C89" s="33"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
       <c r="G89" s="3">
         <v>3.11</v>
       </c>
       <c r="H89" s="3"/>
-      <c r="I89" s="34"/>
-      <c r="J89" s="34"/>
-      <c r="K89" s="34"/>
+      <c r="I89" s="33"/>
+      <c r="J89" s="33"/>
+      <c r="K89" s="33"/>
       <c r="L89" s="3">
         <v>0</v>
       </c>
@@ -5073,25 +5070,25 @@
       <c r="N89" s="3">
         <v>0</v>
       </c>
-      <c r="O89" s="34"/>
-      <c r="P89" s="34"/>
-      <c r="Q89" s="34"/>
-      <c r="R89" s="34"/>
+      <c r="O89" s="33"/>
+      <c r="P89" s="33"/>
+      <c r="Q89" s="33"/>
+      <c r="R89" s="33"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A90" s="34"/>
-      <c r="B90" s="34"/>
-      <c r="C90" s="34"/>
-      <c r="D90" s="34"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="34"/>
+      <c r="A90" s="33"/>
+      <c r="B90" s="33"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="33"/>
       <c r="G90" s="3">
         <v>1.98</v>
       </c>
       <c r="H90" s="3"/>
-      <c r="I90" s="34"/>
-      <c r="J90" s="34"/>
-      <c r="K90" s="34"/>
+      <c r="I90" s="33"/>
+      <c r="J90" s="33"/>
+      <c r="K90" s="33"/>
       <c r="L90" s="3">
         <v>18</v>
       </c>
@@ -5101,63 +5098,124 @@
       <c r="N90" s="3">
         <v>0</v>
       </c>
-      <c r="O90" s="34"/>
-      <c r="P90" s="34"/>
-      <c r="Q90" s="34"/>
-      <c r="R90" s="34"/>
+      <c r="O90" s="33"/>
+      <c r="P90" s="33"/>
+      <c r="Q90" s="33"/>
+      <c r="R90" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="185">
-    <mergeCell ref="J6:J10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F11:F15"/>
-    <mergeCell ref="G11:G15"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="G6:G10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J11:J15"/>
-    <mergeCell ref="K11:K15"/>
-    <mergeCell ref="K17:K21"/>
-    <mergeCell ref="R17:R21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="G22:G26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="F17:F21"/>
-    <mergeCell ref="G17:G21"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="J27:J31"/>
+    <mergeCell ref="F87:F90"/>
+    <mergeCell ref="I87:I90"/>
+    <mergeCell ref="J87:J90"/>
+    <mergeCell ref="K87:K90"/>
+    <mergeCell ref="O87:R90"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="G82:G86"/>
+    <mergeCell ref="I82:I86"/>
+    <mergeCell ref="J82:J86"/>
+    <mergeCell ref="K82:K86"/>
+    <mergeCell ref="R82:R86"/>
+    <mergeCell ref="F82:F86"/>
+    <mergeCell ref="F77:F81"/>
+    <mergeCell ref="G77:G81"/>
+    <mergeCell ref="I77:I81"/>
+    <mergeCell ref="J77:J81"/>
+    <mergeCell ref="K77:K81"/>
+    <mergeCell ref="R77:R81"/>
+    <mergeCell ref="F72:F76"/>
+    <mergeCell ref="G72:G76"/>
+    <mergeCell ref="I72:I76"/>
+    <mergeCell ref="J72:J76"/>
+    <mergeCell ref="K72:K76"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:D90"/>
+    <mergeCell ref="E87:E90"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="D82:D86"/>
+    <mergeCell ref="E82:E86"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="C77:C81"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="E77:E81"/>
+    <mergeCell ref="G67:G71"/>
+    <mergeCell ref="I67:I71"/>
+    <mergeCell ref="J67:J71"/>
+    <mergeCell ref="K67:K71"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="C62:C66"/>
+    <mergeCell ref="D62:D66"/>
+    <mergeCell ref="E62:E66"/>
+    <mergeCell ref="F62:F66"/>
+    <mergeCell ref="R67:R71"/>
+    <mergeCell ref="A72:A76"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="C72:C76"/>
+    <mergeCell ref="D72:D76"/>
+    <mergeCell ref="E72:E76"/>
+    <mergeCell ref="G62:G66"/>
+    <mergeCell ref="I62:I66"/>
+    <mergeCell ref="J62:J66"/>
+    <mergeCell ref="K62:K66"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="C67:C71"/>
+    <mergeCell ref="D67:D71"/>
+    <mergeCell ref="E67:E71"/>
+    <mergeCell ref="F67:F71"/>
+    <mergeCell ref="R52:R56"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="E57:E61"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="I57:I61"/>
+    <mergeCell ref="J57:J61"/>
+    <mergeCell ref="K57:K61"/>
+    <mergeCell ref="R57:R61"/>
+    <mergeCell ref="Q47:Q51"/>
+    <mergeCell ref="R47:R51"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="D52:D56"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="F52:F56"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="I52:I56"/>
+    <mergeCell ref="G47:G51"/>
+    <mergeCell ref="I47:I51"/>
+    <mergeCell ref="J47:J51"/>
+    <mergeCell ref="K47:K51"/>
+    <mergeCell ref="O47:O51"/>
+    <mergeCell ref="P47:P51"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="C47:C51"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="E47:E51"/>
+    <mergeCell ref="F47:F51"/>
+    <mergeCell ref="J52:J56"/>
+    <mergeCell ref="K52:K56"/>
+    <mergeCell ref="G42:G46"/>
+    <mergeCell ref="I42:I46"/>
+    <mergeCell ref="J42:J46"/>
+    <mergeCell ref="K42:K46"/>
+    <mergeCell ref="R42:R46"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="J37:J41"/>
+    <mergeCell ref="K37:K41"/>
+    <mergeCell ref="R37:R41"/>
     <mergeCell ref="K27:K31"/>
     <mergeCell ref="R27:R31"/>
     <mergeCell ref="A32:A36"/>
@@ -5182,117 +5240,56 @@
     <mergeCell ref="E37:E41"/>
     <mergeCell ref="F37:F41"/>
     <mergeCell ref="F42:F46"/>
-    <mergeCell ref="G42:G46"/>
-    <mergeCell ref="I42:I46"/>
-    <mergeCell ref="J42:J46"/>
-    <mergeCell ref="K42:K46"/>
-    <mergeCell ref="R42:R46"/>
-    <mergeCell ref="G37:G41"/>
-    <mergeCell ref="I37:I41"/>
-    <mergeCell ref="J37:J41"/>
-    <mergeCell ref="K37:K41"/>
-    <mergeCell ref="R37:R41"/>
-    <mergeCell ref="Q47:Q51"/>
-    <mergeCell ref="R47:R51"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="D52:D56"/>
-    <mergeCell ref="E52:E56"/>
-    <mergeCell ref="F52:F56"/>
-    <mergeCell ref="G52:G56"/>
-    <mergeCell ref="I52:I56"/>
-    <mergeCell ref="G47:G51"/>
-    <mergeCell ref="I47:I51"/>
-    <mergeCell ref="J47:J51"/>
-    <mergeCell ref="K47:K51"/>
-    <mergeCell ref="O47:O51"/>
-    <mergeCell ref="P47:P51"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="D47:D51"/>
-    <mergeCell ref="E47:E51"/>
-    <mergeCell ref="F47:F51"/>
-    <mergeCell ref="J52:J56"/>
-    <mergeCell ref="K52:K56"/>
-    <mergeCell ref="R52:R56"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="E57:E61"/>
-    <mergeCell ref="F57:F61"/>
-    <mergeCell ref="G57:G61"/>
-    <mergeCell ref="I57:I61"/>
-    <mergeCell ref="J57:J61"/>
-    <mergeCell ref="K57:K61"/>
-    <mergeCell ref="R57:R61"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="C62:C66"/>
-    <mergeCell ref="D62:D66"/>
-    <mergeCell ref="E62:E66"/>
-    <mergeCell ref="F62:F66"/>
-    <mergeCell ref="R67:R71"/>
-    <mergeCell ref="A72:A76"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="C72:C76"/>
-    <mergeCell ref="D72:D76"/>
-    <mergeCell ref="E72:E76"/>
-    <mergeCell ref="G62:G66"/>
-    <mergeCell ref="I62:I66"/>
-    <mergeCell ref="J62:J66"/>
-    <mergeCell ref="K62:K66"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="C67:C71"/>
-    <mergeCell ref="D67:D71"/>
-    <mergeCell ref="E67:E71"/>
-    <mergeCell ref="F67:F71"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="C77:C81"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="E77:E81"/>
-    <mergeCell ref="G67:G71"/>
-    <mergeCell ref="I67:I71"/>
-    <mergeCell ref="J67:J71"/>
-    <mergeCell ref="K67:K71"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="C87:C90"/>
-    <mergeCell ref="D87:D90"/>
-    <mergeCell ref="E87:E90"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="E82:E86"/>
-    <mergeCell ref="F87:F90"/>
-    <mergeCell ref="I87:I90"/>
-    <mergeCell ref="J87:J90"/>
-    <mergeCell ref="K87:K90"/>
-    <mergeCell ref="O87:R90"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="G82:G86"/>
-    <mergeCell ref="I82:I86"/>
-    <mergeCell ref="J82:J86"/>
-    <mergeCell ref="K82:K86"/>
-    <mergeCell ref="R82:R86"/>
-    <mergeCell ref="F82:F86"/>
-    <mergeCell ref="F77:F81"/>
-    <mergeCell ref="G77:G81"/>
-    <mergeCell ref="I77:I81"/>
-    <mergeCell ref="J77:J81"/>
-    <mergeCell ref="K77:K81"/>
-    <mergeCell ref="R77:R81"/>
-    <mergeCell ref="F72:F76"/>
-    <mergeCell ref="G72:G76"/>
-    <mergeCell ref="I72:I76"/>
-    <mergeCell ref="J72:J76"/>
-    <mergeCell ref="K72:K76"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="J27:J31"/>
+    <mergeCell ref="K17:K21"/>
+    <mergeCell ref="R17:R21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="K22:K26"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="E17:E21"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="J6:J10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J11:J15"/>
+    <mergeCell ref="K11:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5305,7 +5302,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5320,22 +5317,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
         <v>198</v>
       </c>
       <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
         <v>199</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>200</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>201</v>
-      </c>
-      <c r="F1" t="s">
-        <v>202</v>
       </c>
       <c r="G1" t="s">
         <v>85</v>
@@ -5344,10 +5341,10 @@
         <v>86</v>
       </c>
       <c r="I1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J1" t="s">
         <v>194</v>
-      </c>
-      <c r="J1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -5872,7 +5869,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5899,10 +5896,10 @@
         <v>176</v>
       </c>
       <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
         <v>192</v>
-      </c>
-      <c r="D1" t="s">
-        <v>193</v>
       </c>
       <c r="E1" t="s">
         <v>177</v>
@@ -5917,10 +5914,10 @@
         <v>180</v>
       </c>
       <c r="I1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J1" t="s">
         <v>190</v>
-      </c>
-      <c r="J1" t="s">
-        <v>191</v>
       </c>
       <c r="K1" t="s">
         <v>181</v>
@@ -6108,7 +6105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9B39B0-AFBE-1848-97F5-4C3DEB224DB7}">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6119,16 +6118,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
         <v>188</v>
       </c>
       <c r="C1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change names in dataset
</commit_message>
<xml_diff>
--- a/static/mock/AntiBio1.xlsx
+++ b/static/mock/AntiBio1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/PycharmProjects/ChemML/static/mock/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/ProgProjects/ChemML/static/mock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E4C666-9A8A-3F47-9549-CA0C3D5CDF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCC5DB7-01C5-9742-843C-29040F4941C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{C97C895C-21C5-4ABD-B085-E1322DB1066B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{C97C895C-21C5-4ABD-B085-E1322DB1066B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="205">
   <si>
     <t>RE</t>
   </si>
@@ -698,19 +698,28 @@
     <t>Is salt</t>
   </si>
   <si>
-    <t xml:space="preserve">Ionic radii </t>
-  </si>
-  <si>
-    <t>Crystal structure type</t>
-  </si>
-  <si>
-    <t>Coordination number salt</t>
-  </si>
-  <si>
-    <t>Coordination number solution</t>
-  </si>
-  <si>
     <t>Stunting diameter</t>
+  </si>
+  <si>
+    <t>Ionic radii RE (salt)</t>
+  </si>
+  <si>
+    <t>Electronegativity (Oganov)</t>
+  </si>
+  <si>
+    <t>Crystal structure type (salt)</t>
+  </si>
+  <si>
+    <t>Coordination number RE (salt)</t>
+  </si>
+  <si>
+    <t>Coordination number RE (solution)</t>
+  </si>
+  <si>
+    <t>рН (solution)</t>
+  </si>
+  <si>
+    <t>Nitrate complexes stability constant (solution)</t>
   </si>
 </sst>
 </file>
@@ -1490,13 +1499,13 @@
   <autoFilter ref="A1:J17" xr:uid="{2D3940D9-BD75-417D-B939-9D9F2B046451}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{6E3D35CA-3D70-45F1-9A50-18CBC54E9741}" name="REE" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{48794F88-A244-474D-A6B2-9FD63736CE7C}" name="Ionic radii " dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{DDE4413E-B094-4AFB-8138-A9932CA5D9D5}" name="Electronegativity" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{CFF1D428-BCF1-46DF-ACB8-4EBDDD164153}" name="Crystal structure type" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{0CA5AF80-08A7-4ED3-B39B-40669072521C}" name="Coordination number salt" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{7FF2FE3D-DBC7-4F57-8794-C0C32F373CE2}" name="Coordination number solution" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{3D5263EB-1B80-41C2-A1C6-35780FE385CD}" name="рН" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{706A363A-7093-4406-B661-54FFDBA06FE1}" name="lgβ" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{48794F88-A244-474D-A6B2-9FD63736CE7C}" name="Ionic radii RE (salt)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{DDE4413E-B094-4AFB-8138-A9932CA5D9D5}" name="Electronegativity (Oganov)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{CFF1D428-BCF1-46DF-ACB8-4EBDDD164153}" name="Crystal structure type (salt)" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{0CA5AF80-08A7-4ED3-B39B-40669072521C}" name="Coordination number RE (salt)" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{7FF2FE3D-DBC7-4F57-8794-C0C32F373CE2}" name="Coordination number RE (solution)" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{3D5263EB-1B80-41C2-A1C6-35780FE385CD}" name="рН (solution)" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{706A363A-7093-4406-B661-54FFDBA06FE1}" name="Nitrate complexes stability constant (solution)" dataDxfId="12"/>
     <tableColumn id="9" xr3:uid="{0FBAAE01-3DD2-4C00-AB7B-8504825C4F0D}" name="Electronic structure RE3+" dataDxfId="11"/>
     <tableColumn id="10" xr3:uid="{B0E7A464-1AB1-4388-AB3A-CABA8176ED5D}" name="Price" dataDxfId="10"/>
   </tableColumns>
@@ -5301,13 +5310,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FB0CCE-FF23-4E20-9F55-6D7C26036CC2}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" customWidth="1"/>
@@ -5320,25 +5329,25 @@
         <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>199</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G1" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
       <c r="H1" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="I1" t="s">
         <v>193</v>
@@ -6105,7 +6114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9B39B0-AFBE-1848-97F5-4C3DEB224DB7}">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -6127,7 +6136,7 @@
         <v>196</v>
       </c>
       <c r="D1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>